<commit_message>
Updated Grid Battery Storage Capacity to 500 GW after consultation with Mike and looking at 2035 report/scenario
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\elec\GBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A638F84-8FA8-49E7-8310-4C7EBB4F24E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="60" windowWidth="21615" windowHeight="16485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="60" windowWidth="21615" windowHeight="16485" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
   <definedNames>
     <definedName name="gigwatts_to_megawatts">About!$A$32</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,14 +38,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -61,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="178">
   <si>
     <t>Source:</t>
   </si>
@@ -492,27 +491,12 @@
     <t>Potential Additional Battery Storage Capacity</t>
   </si>
   <si>
-    <t>National Renewable Energy Laboratory</t>
-  </si>
-  <si>
-    <t>https://www.nrel.gov/analysis/re_futures/data_viewer/</t>
-  </si>
-  <si>
-    <t>Renewable Electricity Futures Scenario Viewer</t>
-  </si>
-  <si>
-    <t>"80% RE-ITI (2014)" scenario</t>
-  </si>
-  <si>
     <t>GW</t>
   </si>
   <si>
     <t>Battery Storage Capacity</t>
   </si>
   <si>
-    <t>80% RE-ITI (2014) scenario</t>
-  </si>
-  <si>
     <t>BAU scenario</t>
   </si>
   <si>
@@ -525,9 +509,6 @@
     <t>from present-day values to the 2050 value utilized in the 80% RE-ITI (2014) scenario.</t>
   </si>
   <si>
-    <t>2012 (data revised 2014)</t>
-  </si>
-  <si>
     <t>AEO BAU</t>
   </si>
   <si>
@@ -537,9 +518,6 @@
     <t>Additional Potential</t>
   </si>
   <si>
-    <t>NREL 80% RE-ITI annualized</t>
-  </si>
-  <si>
     <t>Unit Conversion</t>
   </si>
   <si>
@@ -601,12 +579,27 @@
   </si>
   <si>
     <t>GBSC Start Year Grid Battery Storage Capacity</t>
+  </si>
+  <si>
+    <t>GSPP, GridLab, Energy Innovation</t>
+  </si>
+  <si>
+    <t>The 2035 Report</t>
+  </si>
+  <si>
+    <t>https://www.2035report.com/data-explorer/</t>
+  </si>
+  <si>
+    <t>2034 Report Annualized</t>
+  </si>
+  <si>
+    <t>2035 Scenario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
@@ -1185,64 +1178,64 @@
     </xf>
   </cellXfs>
   <cellStyles count="58">
-    <cellStyle name="20% - Accent1 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Body: normal cell" xfId="56" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Calculation 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Check Cell 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Euro" xfId="30" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="52" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="57" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Good 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Header: bottom row" xfId="53" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Heading 1 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Heading 2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Heading 3 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Heading 4 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="3"/>
+    <cellStyle name="20% - Accent2 2" xfId="4"/>
+    <cellStyle name="20% - Accent3 2" xfId="5"/>
+    <cellStyle name="20% - Accent4 2" xfId="6"/>
+    <cellStyle name="20% - Accent5 2" xfId="7"/>
+    <cellStyle name="20% - Accent6 2" xfId="8"/>
+    <cellStyle name="40% - Accent1 2" xfId="9"/>
+    <cellStyle name="40% - Accent2 2" xfId="10"/>
+    <cellStyle name="40% - Accent3 2" xfId="11"/>
+    <cellStyle name="40% - Accent4 2" xfId="12"/>
+    <cellStyle name="40% - Accent5 2" xfId="13"/>
+    <cellStyle name="40% - Accent6 2" xfId="14"/>
+    <cellStyle name="60% - Accent1 2" xfId="15"/>
+    <cellStyle name="60% - Accent2 2" xfId="16"/>
+    <cellStyle name="60% - Accent3 2" xfId="17"/>
+    <cellStyle name="60% - Accent4 2" xfId="18"/>
+    <cellStyle name="60% - Accent5 2" xfId="19"/>
+    <cellStyle name="60% - Accent6 2" xfId="20"/>
+    <cellStyle name="Accent1 2" xfId="21"/>
+    <cellStyle name="Accent2 2" xfId="22"/>
+    <cellStyle name="Accent3 2" xfId="23"/>
+    <cellStyle name="Accent4 2" xfId="24"/>
+    <cellStyle name="Accent5 2" xfId="25"/>
+    <cellStyle name="Accent6 2" xfId="26"/>
+    <cellStyle name="Bad 2" xfId="27"/>
+    <cellStyle name="Body: normal cell" xfId="56"/>
+    <cellStyle name="Calculation 2" xfId="28"/>
+    <cellStyle name="Check Cell 2" xfId="29"/>
+    <cellStyle name="Euro" xfId="30"/>
+    <cellStyle name="Explanatory Text 2" xfId="31"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="52"/>
+    <cellStyle name="Footnotes: top row" xfId="57"/>
+    <cellStyle name="Good 2" xfId="32"/>
+    <cellStyle name="Header: bottom row" xfId="53"/>
+    <cellStyle name="Heading 1 2" xfId="33"/>
+    <cellStyle name="Heading 2 2" xfId="34"/>
+    <cellStyle name="Heading 3 2" xfId="35"/>
+    <cellStyle name="Heading 4 2" xfId="36"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Input 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Neutral 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Input 2" xfId="37"/>
+    <cellStyle name="Linked Cell 2" xfId="38"/>
+    <cellStyle name="Neutral 2" xfId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Normal 2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Normal 2 3" xfId="48" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Normal 2 4" xfId="49" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Normal 2 5" xfId="50" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Normal 2 6" xfId="51" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Normal 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Normal 4" xfId="47" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Note 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Output 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Parent row" xfId="55" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Table title" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Title 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Total 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Warning Text 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="45"/>
+    <cellStyle name="Normal 2 3" xfId="48"/>
+    <cellStyle name="Normal 2 4" xfId="49"/>
+    <cellStyle name="Normal 2 5" xfId="50"/>
+    <cellStyle name="Normal 2 6" xfId="51"/>
+    <cellStyle name="Normal 3" xfId="46"/>
+    <cellStyle name="Normal 4" xfId="47"/>
+    <cellStyle name="Note 2" xfId="40"/>
+    <cellStyle name="Output 2" xfId="41"/>
+    <cellStyle name="Parent row" xfId="55"/>
+    <cellStyle name="Table title" xfId="54"/>
+    <cellStyle name="Title 2" xfId="42"/>
+    <cellStyle name="Total 2" xfId="43"/>
+    <cellStyle name="Warning Text 2" xfId="44"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1333,23 +1326,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1385,23 +1361,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1577,10 +1536,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1600,7 +1561,7 @@
     </row>
     <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1643,35 +1604,31 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
-        <v>154</v>
+      <c r="B14" s="27">
+        <v>2020</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1686,7 +1643,7 @@
     </row>
     <row r="22" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1715,12 +1672,12 @@
     </row>
     <row r="29" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1733,17 +1690,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{4AAB35F3-E4EE-4CDD-8B90-E66DDAE1B1CB}"/>
-    <hyperlink ref="B23" r:id="rId3" xr:uid="{25D49C5B-9071-4F47-BE96-21550C23981D}"/>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B23" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI114"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
@@ -8651,7 +8607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE298A7-64E3-4A08-A1AD-13DAF221318C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK114"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -8669,7 +8625,7 @@
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="13" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C1" s="14">
         <v>2017</v>
@@ -8780,7 +8736,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -8791,7 +8747,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -8804,7 +8760,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -8816,7 +8772,7 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -8941,7 +8897,7 @@
         <v>12</v>
       </c>
       <c r="AK12" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13492,7 +13448,7 @@
         <v>74</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C60" s="20" t="s">
         <v>36</v>
@@ -15835,7 +15791,7 @@
     </row>
     <row r="95" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15865,12 +15821,12 @@
     </row>
     <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="11" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15905,32 +15861,32 @@
     </row>
     <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="11" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="11" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="11" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="11" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="114" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="11" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -15942,10 +15898,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3557BBA5-03BB-4AA1-A8BA-0CA4E738B5D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15954,49 +15912,50 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="7">
-        <v>2050</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3">
-        <v>26</v>
+        <v>145</v>
+      </c>
+      <c r="B3" s="8">
+        <f>BGBSC!R2/10^3</f>
+        <v>10.804548</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="B4">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -16006,7 +15965,7 @@
     </row>
     <row r="12" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B12" s="6">
         <f>'AEO Table 9'!C23</f>
@@ -16024,15 +15983,14 @@
     </row>
     <row r="15" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B15" s="6">
         <f>B12</f>
         <v>1.3702000000000001</v>
       </c>
       <c r="C15" s="6">
-        <f>B4</f>
-        <v>120</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -16136,140 +16094,140 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="B18" s="28" cm="1">
         <f t="array" ref="B18">TREND($B$15:$C$15,$B$14:$C$14,B$17)</f>
-        <v>1.3701999999993859</v>
+        <v>1.3701999999975669</v>
       </c>
       <c r="C18" s="28" cm="1">
         <f t="array" ref="C18">TREND($B$15:$C$15,$B$14:$C$14,C$17)</f>
-        <v>5.1969677419347136</v>
+        <v>17.455032258061692</v>
       </c>
       <c r="D18" s="28" cm="1">
         <f t="array" ref="D18">TREND($B$15:$C$15,$B$14:$C$14,D$17)</f>
-        <v>9.0237354838700412</v>
+        <v>33.539864516125817</v>
       </c>
       <c r="E18" s="28" cm="1">
         <f t="array" ref="E18">TREND($B$15:$C$15,$B$14:$C$14,E$17)</f>
-        <v>12.850503225806278</v>
+        <v>49.624696774189943</v>
       </c>
       <c r="F18" s="28" cm="1">
         <f t="array" ref="F18">TREND($B$15:$C$15,$B$14:$C$14,F$17)</f>
-        <v>16.677270967741606</v>
+        <v>65.709529032254068</v>
       </c>
       <c r="G18" s="28" cm="1">
         <f t="array" ref="G18">TREND($B$15:$C$15,$B$14:$C$14,G$17)</f>
-        <v>20.504038709676934</v>
+        <v>81.794361290318193</v>
       </c>
       <c r="H18" s="28" cm="1">
         <f t="array" ref="H18">TREND($B$15:$C$15,$B$14:$C$14,H$17)</f>
-        <v>24.330806451612261</v>
+        <v>97.879193548385956</v>
       </c>
       <c r="I18" s="28" cm="1">
         <f t="array" ref="I18">TREND($B$15:$C$15,$B$14:$C$14,I$17)</f>
-        <v>28.157574193547589</v>
+        <v>113.96402580645008</v>
       </c>
       <c r="J18" s="28" cm="1">
         <f t="array" ref="J18">TREND($B$15:$C$15,$B$14:$C$14,J$17)</f>
-        <v>31.984341935482917</v>
+        <v>130.04885806451421</v>
       </c>
       <c r="K18" s="28" cm="1">
         <f t="array" ref="K18">TREND($B$15:$C$15,$B$14:$C$14,K$17)</f>
-        <v>35.811109677419154</v>
+        <v>146.13369032257833</v>
       </c>
       <c r="L18" s="28" cm="1">
         <f t="array" ref="L18">TREND($B$15:$C$15,$B$14:$C$14,L$17)</f>
-        <v>39.637877419354481</v>
+        <v>162.21852258064246</v>
       </c>
       <c r="M18" s="28" cm="1">
         <f t="array" ref="M18">TREND($B$15:$C$15,$B$14:$C$14,M$17)</f>
-        <v>43.464645161289809</v>
+        <v>178.30335483870658</v>
       </c>
       <c r="N18" s="28" cm="1">
         <f t="array" ref="N18">TREND($B$15:$C$15,$B$14:$C$14,N$17)</f>
-        <v>47.291412903225137</v>
+        <v>194.38818709677071</v>
       </c>
       <c r="O18" s="28" cm="1">
         <f t="array" ref="O18">TREND($B$15:$C$15,$B$14:$C$14,O$17)</f>
-        <v>51.118180645160464</v>
+        <v>210.47301935483483</v>
       </c>
       <c r="P18" s="28" cm="1">
         <f t="array" ref="P18">TREND($B$15:$C$15,$B$14:$C$14,P$17)</f>
-        <v>54.944948387095792</v>
+        <v>226.55785161289896</v>
       </c>
       <c r="Q18" s="28" cm="1">
         <f t="array" ref="Q18">TREND($B$15:$C$15,$B$14:$C$14,Q$17)</f>
-        <v>58.771716129032029</v>
+        <v>242.64268387096672</v>
       </c>
       <c r="R18" s="28" cm="1">
         <f t="array" ref="R18">TREND($B$15:$C$15,$B$14:$C$14,R$17)</f>
-        <v>62.598483870967357</v>
+        <v>258.72751612903085</v>
       </c>
       <c r="S18" s="28" cm="1">
         <f t="array" ref="S18">TREND($B$15:$C$15,$B$14:$C$14,S$17)</f>
-        <v>66.425251612902684</v>
+        <v>274.81234838709497</v>
       </c>
       <c r="T18" s="28" cm="1">
         <f t="array" ref="T18">TREND($B$15:$C$15,$B$14:$C$14,T$17)</f>
-        <v>70.252019354838012</v>
+        <v>290.8971806451591</v>
       </c>
       <c r="U18" s="28" cm="1">
         <f t="array" ref="U18">TREND($B$15:$C$15,$B$14:$C$14,U$17)</f>
-        <v>74.07878709677334</v>
+        <v>306.98201290321958</v>
       </c>
       <c r="V18" s="28" cm="1">
         <f t="array" ref="V18">TREND($B$15:$C$15,$B$14:$C$14,V$17)</f>
-        <v>77.905554838708667</v>
+        <v>323.06684516129098</v>
       </c>
       <c r="W18" s="28" cm="1">
         <f t="array" ref="W18">TREND($B$15:$C$15,$B$14:$C$14,W$17)</f>
-        <v>81.732322580644905</v>
+        <v>339.15167741935511</v>
       </c>
       <c r="X18" s="28" cm="1">
         <f t="array" ref="X18">TREND($B$15:$C$15,$B$14:$C$14,X$17)</f>
-        <v>85.559090322580232</v>
+        <v>355.23650967741924</v>
       </c>
       <c r="Y18" s="28" cm="1">
         <f t="array" ref="Y18">TREND($B$15:$C$15,$B$14:$C$14,Y$17)</f>
-        <v>89.38585806451556</v>
+        <v>371.32134193548336</v>
       </c>
       <c r="Z18" s="28" cm="1">
         <f t="array" ref="Z18">TREND($B$15:$C$15,$B$14:$C$14,Z$17)</f>
-        <v>93.212625806450887</v>
+        <v>387.40617419354749</v>
       </c>
       <c r="AA18" s="28" cm="1">
         <f t="array" ref="AA18">TREND($B$15:$C$15,$B$14:$C$14,AA$17)</f>
-        <v>97.039393548386215</v>
+        <v>403.49100645161161</v>
       </c>
       <c r="AB18" s="28" cm="1">
         <f t="array" ref="AB18">TREND($B$15:$C$15,$B$14:$C$14,AB$17)</f>
-        <v>100.86616129032154</v>
+        <v>419.57583870967574</v>
       </c>
       <c r="AC18" s="28" cm="1">
         <f t="array" ref="AC18">TREND($B$15:$C$15,$B$14:$C$14,AC$17)</f>
-        <v>104.69292903225778</v>
+        <v>435.66067096773986</v>
       </c>
       <c r="AD18" s="28" cm="1">
         <f t="array" ref="AD18">TREND($B$15:$C$15,$B$14:$C$14,AD$17)</f>
-        <v>108.51969677419311</v>
+        <v>451.74550322580399</v>
       </c>
       <c r="AE18" s="28" cm="1">
         <f t="array" ref="AE18">TREND($B$15:$C$15,$B$14:$C$14,AE$17)</f>
-        <v>112.34646451612844</v>
+        <v>467.83033548386811</v>
       </c>
       <c r="AF18" s="28" cm="1">
         <f t="array" ref="AF18">TREND($B$15:$C$15,$B$14:$C$14,AF$17)</f>
-        <v>116.17323225806376</v>
+        <v>483.91516774193224</v>
       </c>
       <c r="AG18" s="28" cm="1">
         <f t="array" ref="AG18">TREND($B$15:$C$15,$B$14:$C$14,AG$17)</f>
-        <v>119.99999999999909</v>
+        <v>499.99999999999636</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B19" s="28">
         <f>'AEO Table 9'!C23</f>
@@ -16402,135 +16360,135 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B20" s="30">
         <f>B18-B19</f>
-        <v>-6.141753772226366E-13</v>
+        <v>-2.4331647807684931E-12</v>
       </c>
       <c r="C20" s="30">
         <f t="shared" ref="C20:AG20" si="0">C18-C19</f>
-        <v>2.5681077419347136</v>
+        <v>14.826172258061693</v>
       </c>
       <c r="D20" s="30">
         <f t="shared" si="0"/>
-        <v>3.3948754838700408</v>
+        <v>27.911004516125818</v>
       </c>
       <c r="E20" s="30">
         <f t="shared" si="0"/>
-        <v>6.5906432258062786</v>
+        <v>43.364836774189939</v>
       </c>
       <c r="F20" s="30">
         <f t="shared" si="0"/>
-        <v>9.786409967741605</v>
+        <v>58.818668032254067</v>
       </c>
       <c r="G20" s="30">
         <f t="shared" si="0"/>
-        <v>12.983177709676934</v>
+        <v>74.273500290318196</v>
       </c>
       <c r="H20" s="30">
         <f t="shared" si="0"/>
-        <v>16.36694545161226</v>
+        <v>89.915332548385962</v>
       </c>
       <c r="I20" s="30">
         <f t="shared" si="0"/>
-        <v>19.78271319354759</v>
+        <v>105.58916480645009</v>
       </c>
       <c r="J20" s="30">
         <f t="shared" si="0"/>
-        <v>23.198480935482916</v>
+        <v>121.26299706451421</v>
       </c>
       <c r="K20" s="30">
         <f t="shared" si="0"/>
-        <v>26.614248677419155</v>
+        <v>136.93682932257832</v>
       </c>
       <c r="L20" s="30">
         <f t="shared" si="0"/>
-        <v>29.979035419354481</v>
+        <v>152.55968058064246</v>
       </c>
       <c r="M20" s="30">
         <f t="shared" si="0"/>
-        <v>33.394803161289808</v>
+        <v>168.23351283870659</v>
       </c>
       <c r="N20" s="30">
         <f t="shared" si="0"/>
-        <v>37.221570903225135</v>
+        <v>184.31834509677071</v>
       </c>
       <c r="O20" s="30">
         <f t="shared" si="0"/>
-        <v>41.048338645160463</v>
+        <v>200.40317735483484</v>
       </c>
       <c r="P20" s="30">
         <f t="shared" si="0"/>
-        <v>44.588082387095795</v>
+        <v>216.20098561289896</v>
       </c>
       <c r="Q20" s="30">
         <f t="shared" si="0"/>
-        <v>47.967168129032032</v>
+        <v>231.83813587096671</v>
       </c>
       <c r="R20" s="30">
         <f t="shared" si="0"/>
-        <v>51.79393587096736</v>
+        <v>247.92296812903083</v>
       </c>
       <c r="S20" s="30">
         <f t="shared" si="0"/>
-        <v>55.553119612902684</v>
+        <v>263.94021638709495</v>
       </c>
       <c r="T20" s="30">
         <f t="shared" si="0"/>
-        <v>59.379887354838012</v>
+        <v>280.02504864515907</v>
       </c>
       <c r="U20" s="30">
         <f t="shared" si="0"/>
-        <v>63.191855096773338</v>
+        <v>296.09508090321958</v>
       </c>
       <c r="V20" s="30">
         <f t="shared" si="0"/>
-        <v>67.018622838708666</v>
+        <v>312.17991316129098</v>
       </c>
       <c r="W20" s="30">
         <f t="shared" si="0"/>
-        <v>70.7580415806449</v>
+        <v>328.17739641935509</v>
       </c>
       <c r="X20" s="30">
         <f t="shared" si="0"/>
-        <v>74.145410322580233</v>
+        <v>343.82282967741924</v>
       </c>
       <c r="Y20" s="30">
         <f t="shared" si="0"/>
-        <v>77.377454064515561</v>
+        <v>359.31293793548338</v>
       </c>
       <c r="Z20" s="30">
         <f t="shared" si="0"/>
-        <v>81.204221806450889</v>
+        <v>375.3977701935475</v>
       </c>
       <c r="AA20" s="30">
         <f t="shared" si="0"/>
-        <v>85.030989548386216</v>
+        <v>391.48260245161163</v>
       </c>
       <c r="AB20" s="30">
         <f t="shared" si="0"/>
-        <v>88.223900290321538</v>
+        <v>406.93357770967572</v>
       </c>
       <c r="AC20" s="30">
         <f t="shared" si="0"/>
-        <v>91.371272032257778</v>
+        <v>422.33901396773985</v>
       </c>
       <c r="AD20" s="30">
         <f t="shared" si="0"/>
-        <v>93.438023774193113</v>
+        <v>436.66383022580396</v>
       </c>
       <c r="AE20" s="30">
         <f t="shared" si="0"/>
-        <v>96.26378251612843</v>
+        <v>451.74765348386813</v>
       </c>
       <c r="AF20" s="30">
         <f t="shared" si="0"/>
-        <v>98.807126258063761</v>
+        <v>466.54906174193223</v>
       </c>
       <c r="AG20" s="30">
         <f t="shared" si="0"/>
-        <v>102.59910399999909</v>
+        <v>482.59910399999637</v>
       </c>
     </row>
   </sheetData>
@@ -16539,7 +16497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -16794,13 +16752,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E930CD6-BDBE-4B51-AE85-855FFBE243D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16916,131 +16874,131 @@
       </c>
       <c r="B2" s="8">
         <f>'RE Futures Data &amp; Calcs'!B20*gigwatts_to_megawatts</f>
-        <v>-6.141753772226366E-10</v>
+        <v>-2.4331647807684931E-9</v>
       </c>
       <c r="C2" s="8">
         <f>'RE Futures Data &amp; Calcs'!C20*gigwatts_to_megawatts</f>
-        <v>2568.1077419347134</v>
+        <v>14826.172258061693</v>
       </c>
       <c r="D2" s="8">
         <f>'RE Futures Data &amp; Calcs'!D20*gigwatts_to_megawatts</f>
-        <v>3394.8754838700406</v>
+        <v>27911.004516125817</v>
       </c>
       <c r="E2" s="8">
         <f>'RE Futures Data &amp; Calcs'!E20*gigwatts_to_megawatts</f>
-        <v>6590.6432258062787</v>
+        <v>43364.836774189942</v>
       </c>
       <c r="F2" s="8">
         <f>'RE Futures Data &amp; Calcs'!F20*gigwatts_to_megawatts</f>
-        <v>9786.4099677416052</v>
+        <v>58818.668032254063</v>
       </c>
       <c r="G2" s="8">
         <f>'RE Futures Data &amp; Calcs'!G20*gigwatts_to_megawatts</f>
-        <v>12983.177709676933</v>
+        <v>74273.500290318203</v>
       </c>
       <c r="H2" s="8">
         <f>'RE Futures Data &amp; Calcs'!H20*gigwatts_to_megawatts</f>
-        <v>16366.945451612261</v>
+        <v>89915.332548385966</v>
       </c>
       <c r="I2" s="8">
         <f>'RE Futures Data &amp; Calcs'!I20*gigwatts_to_megawatts</f>
-        <v>19782.713193547588</v>
+        <v>105589.16480645009</v>
       </c>
       <c r="J2" s="8">
         <f>'RE Futures Data &amp; Calcs'!J20*gigwatts_to_megawatts</f>
-        <v>23198.480935482916</v>
+        <v>121262.99706451422</v>
       </c>
       <c r="K2" s="8">
         <f>'RE Futures Data &amp; Calcs'!K20*gigwatts_to_megawatts</f>
-        <v>26614.248677419157</v>
+        <v>136936.82932257833</v>
       </c>
       <c r="L2" s="8">
         <f>'RE Futures Data &amp; Calcs'!L20*gigwatts_to_megawatts</f>
-        <v>29979.035419354481</v>
+        <v>152559.68058064245</v>
       </c>
       <c r="M2" s="8">
         <f>'RE Futures Data &amp; Calcs'!M20*gigwatts_to_megawatts</f>
-        <v>33394.803161289805</v>
+        <v>168233.51283870658</v>
       </c>
       <c r="N2" s="8">
         <f>'RE Futures Data &amp; Calcs'!N20*gigwatts_to_megawatts</f>
-        <v>37221.570903225132</v>
+        <v>184318.3450967707</v>
       </c>
       <c r="O2" s="8">
         <f>'RE Futures Data &amp; Calcs'!O20*gigwatts_to_megawatts</f>
-        <v>41048.33864516046</v>
+        <v>200403.17735483483</v>
       </c>
       <c r="P2" s="8">
         <f>'RE Futures Data &amp; Calcs'!P20*gigwatts_to_megawatts</f>
-        <v>44588.082387095797</v>
+        <v>216200.98561289895</v>
       </c>
       <c r="Q2" s="8">
         <f>'RE Futures Data &amp; Calcs'!Q20*gigwatts_to_megawatts</f>
-        <v>47967.168129032034</v>
+        <v>231838.13587096671</v>
       </c>
       <c r="R2" s="8">
         <f>'RE Futures Data &amp; Calcs'!R20*gigwatts_to_megawatts</f>
-        <v>51793.935870967362</v>
+        <v>247922.96812903084</v>
       </c>
       <c r="S2" s="8">
         <f>'RE Futures Data &amp; Calcs'!S20*gigwatts_to_megawatts</f>
-        <v>55553.119612902687</v>
+        <v>263940.21638709493</v>
       </c>
       <c r="T2" s="8">
         <f>'RE Futures Data &amp; Calcs'!T20*gigwatts_to_megawatts</f>
-        <v>59379.887354838014</v>
+        <v>280025.04864515906</v>
       </c>
       <c r="U2" s="8">
         <f>'RE Futures Data &amp; Calcs'!U20*gigwatts_to_megawatts</f>
-        <v>63191.855096773339</v>
+        <v>296095.08090321958</v>
       </c>
       <c r="V2" s="8">
         <f>'RE Futures Data &amp; Calcs'!V20*gigwatts_to_megawatts</f>
-        <v>67018.622838708659</v>
+        <v>312179.91316129098</v>
       </c>
       <c r="W2" s="8">
         <f>'RE Futures Data &amp; Calcs'!W20*gigwatts_to_megawatts</f>
-        <v>70758.041580644902</v>
+        <v>328177.39641935506</v>
       </c>
       <c r="X2" s="8">
         <f>'RE Futures Data &amp; Calcs'!X20*gigwatts_to_megawatts</f>
-        <v>74145.410322580239</v>
+        <v>343822.82967741921</v>
       </c>
       <c r="Y2" s="8">
         <f>'RE Futures Data &amp; Calcs'!Y20*gigwatts_to_megawatts</f>
-        <v>77377.454064515565</v>
+        <v>359312.93793548335</v>
       </c>
       <c r="Z2" s="8">
         <f>'RE Futures Data &amp; Calcs'!Z20*gigwatts_to_megawatts</f>
-        <v>81204.221806450892</v>
+        <v>375397.77019354748</v>
       </c>
       <c r="AA2" s="8">
         <f>'RE Futures Data &amp; Calcs'!AA20*gigwatts_to_megawatts</f>
-        <v>85030.98954838622</v>
+        <v>391482.6024516116</v>
       </c>
       <c r="AB2" s="8">
         <f>'RE Futures Data &amp; Calcs'!AB20*gigwatts_to_megawatts</f>
-        <v>88223.900290321544</v>
+        <v>406933.57770967571</v>
       </c>
       <c r="AC2" s="8">
         <f>'RE Futures Data &amp; Calcs'!AC20*gigwatts_to_megawatts</f>
-        <v>91371.272032257781</v>
+        <v>422339.01396773983</v>
       </c>
       <c r="AD2" s="8">
         <f>'RE Futures Data &amp; Calcs'!AD20*gigwatts_to_megawatts</f>
-        <v>93438.02377419312</v>
+        <v>436663.83022580395</v>
       </c>
       <c r="AE2" s="8">
         <f>'RE Futures Data &amp; Calcs'!AE20*gigwatts_to_megawatts</f>
-        <v>96263.782516128427</v>
+        <v>451747.65348386811</v>
       </c>
       <c r="AF2" s="8">
         <f>'RE Futures Data &amp; Calcs'!AF20*gigwatts_to_megawatts</f>
-        <v>98807.126258063756</v>
+        <v>466549.06174193224</v>
       </c>
       <c r="AG2" s="8">
         <f>'RE Futures Data &amp; Calcs'!AG20*gigwatts_to_megawatts</f>
-        <v>102599.10399999909</v>
+        <v>482599.10399999638</v>
       </c>
     </row>
   </sheetData>
@@ -17050,7 +17008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59172300-46A9-4F58-8C21-81ABD9E9BA2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -17070,12 +17028,12 @@
         <v>139</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B2" s="5">
         <f>'AEO Table 9 (2019)'!D23*gigwatts_to_megawatts</f>

</xml_diff>

<commit_message>
Update methodology description in GBSC
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\GBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="60" windowWidth="21615" windowHeight="16485" activeTab="5"/>
+    <workbookView xWindow="3975" yWindow="60" windowWidth="21615" windowHeight="16485"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="180">
   <si>
     <t>Source:</t>
   </si>
@@ -500,15 +500,9 @@
     <t>BAU scenario</t>
   </si>
   <si>
-    <t>We use the EIA AEO data as our BAU case, not NREL's RE Futures.</t>
-  </si>
-  <si>
     <t>Additional potential is the difference between the AEO baseline and a linear approach</t>
   </si>
   <si>
-    <t>from present-day values to the 2050 value utilized in the 80% RE-ITI (2014) scenario.</t>
-  </si>
-  <si>
     <t>AEO BAU</t>
   </si>
   <si>
@@ -594,6 +588,18 @@
   </si>
   <si>
     <t>2035 Scenario</t>
+  </si>
+  <si>
+    <t>We use the EIA AEO data as our BAU case.</t>
+  </si>
+  <si>
+    <t>from present-day values to the selected 2050 value. The 2035 Report referenced deploys 150 GW in 2035</t>
+  </si>
+  <si>
+    <t>but only considers a 90% CES and no electrification on top of BAU (and extends only to 2035).</t>
+  </si>
+  <si>
+    <t>Given these consideration, we assume 500 GW can be deployed by 2050.</t>
   </si>
 </sst>
 </file>
@@ -1539,32 +1545,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1572,115 +1578,115 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="3">
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B14" s="27">
         <v>2020</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B20" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B21" s="3">
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B22" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B23" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B24" s="6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="3">
         <v>1000</v>
       </c>
@@ -1704,14 +1710,14 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="42.73046875" style="6" customWidth="1"/>
     <col min="3" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="13" t="s">
         <v>122</v>
       </c>
@@ -1812,14 +1818,14 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
@@ -1830,7 +1836,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
@@ -1854,7 +1860,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
@@ -1865,7 +1871,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="10" t="s">
         <v>9</v>
       </c>
@@ -1873,12 +1879,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
@@ -1982,7 +1988,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
@@ -2086,18 +2092,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>16</v>
       </c>
@@ -2204,7 +2210,7 @@
         <v>-2.0031E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
@@ -2311,7 +2317,7 @@
         <v>-1.3575E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
@@ -2418,7 +2424,7 @@
         <v>1.6708000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
         <v>22</v>
       </c>
@@ -2525,7 +2531,7 @@
         <v>2.7220999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>24</v>
       </c>
@@ -2632,7 +2638,7 @@
         <v>-7.1539999999999998E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
         <v>26</v>
       </c>
@@ -2739,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="22" t="s">
         <v>28</v>
       </c>
@@ -2846,7 +2852,7 @@
         <v>8.5441000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
@@ -2953,7 +2959,7 @@
         <v>1.1962E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
         <v>32</v>
       </c>
@@ -3060,7 +3066,7 @@
         <v>3.1888E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>34</v>
       </c>
@@ -3167,7 +3173,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="10" t="s">
         <v>37</v>
       </c>
@@ -3274,12 +3280,12 @@
         <v>1.5689000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="10" t="s">
         <v>40</v>
       </c>
@@ -3386,7 +3392,7 @@
         <v>-9.4450000000000003E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="10" t="s">
         <v>42</v>
       </c>
@@ -3493,7 +3499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="10" t="s">
         <v>44</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>-2.5900000000000001E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="10" t="s">
         <v>45</v>
       </c>
@@ -3707,7 +3713,7 @@
         <v>-4.9399999999999997E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="10" t="s">
         <v>46</v>
       </c>
@@ -3814,7 +3820,7 @@
         <v>-1.6899999999999999E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="10" t="s">
         <v>47</v>
       </c>
@@ -3921,12 +3927,12 @@
         <v>-1.0089999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="10" t="s">
         <v>49</v>
       </c>
@@ -4033,7 +4039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="10" t="s">
         <v>50</v>
       </c>
@@ -4140,7 +4146,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="10" t="s">
         <v>51</v>
       </c>
@@ -4247,7 +4253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="10" t="s">
         <v>52</v>
       </c>
@@ -4354,7 +4360,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="10" t="s">
         <v>53</v>
       </c>
@@ -4461,7 +4467,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="10" t="s">
         <v>55</v>
       </c>
@@ -4568,7 +4574,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="10" t="s">
         <v>56</v>
       </c>
@@ -4675,7 +4681,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
         <v>57</v>
       </c>
@@ -4782,7 +4788,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="10" t="s">
         <v>58</v>
       </c>
@@ -4889,7 +4895,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="10" t="s">
         <v>59</v>
       </c>
@@ -4996,7 +5002,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="10" t="s">
         <v>61</v>
       </c>
@@ -5103,12 +5109,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="10" t="s">
         <v>63</v>
       </c>
@@ -5215,7 +5221,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="10" t="s">
         <v>64</v>
       </c>
@@ -5322,7 +5328,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="10" t="s">
         <v>65</v>
       </c>
@@ -5429,7 +5435,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="10" t="s">
         <v>66</v>
       </c>
@@ -5536,7 +5542,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="10" t="s">
         <v>67</v>
       </c>
@@ -5643,7 +5649,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="10" t="s">
         <v>68</v>
       </c>
@@ -5750,7 +5756,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="10" t="s">
         <v>69</v>
       </c>
@@ -5857,7 +5863,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="10" t="s">
         <v>70</v>
       </c>
@@ -5964,7 +5970,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="10" t="s">
         <v>71</v>
       </c>
@@ -6071,7 +6077,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="10" t="s">
         <v>72</v>
       </c>
@@ -6178,7 +6184,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="10" t="s">
         <v>73</v>
       </c>
@@ -6285,7 +6291,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="10" t="s">
         <v>74</v>
       </c>
@@ -6392,12 +6398,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="10" t="s">
         <v>76</v>
       </c>
@@ -6504,7 +6510,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="10" t="s">
         <v>77</v>
       </c>
@@ -6611,7 +6617,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="10" t="s">
         <v>78</v>
       </c>
@@ -6718,7 +6724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="10" t="s">
         <v>79</v>
       </c>
@@ -6825,7 +6831,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="10" t="s">
         <v>80</v>
       </c>
@@ -6932,7 +6938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="10" t="s">
         <v>81</v>
       </c>
@@ -7039,7 +7045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="10" t="s">
         <v>82</v>
       </c>
@@ -7146,7 +7152,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="10" t="s">
         <v>83</v>
       </c>
@@ -7253,7 +7259,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="10" t="s">
         <v>84</v>
       </c>
@@ -7360,7 +7366,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="10" t="s">
         <v>85</v>
       </c>
@@ -7467,7 +7473,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="10" t="s">
         <v>86</v>
       </c>
@@ -7574,12 +7580,12 @@
         <v>1.5321E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B76" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="10" t="s">
         <v>89</v>
       </c>
@@ -7686,7 +7692,7 @@
         <v>-1.0508E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="10" t="s">
         <v>90</v>
       </c>
@@ -7793,7 +7799,7 @@
         <v>-2.98E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="10" t="s">
         <v>92</v>
       </c>
@@ -7900,7 +7906,7 @@
         <v>2.3052E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="10" t="s">
         <v>94</v>
       </c>
@@ -8007,7 +8013,7 @@
         <v>-4.7699999999999999E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="10" t="s">
         <v>96</v>
       </c>
@@ -8114,7 +8120,7 @@
         <v>4.6114000000000002E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="10" t="s">
         <v>97</v>
       </c>
@@ -8221,7 +8227,7 @@
         <v>4.542E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="10" t="s">
         <v>99</v>
       </c>
@@ -8328,7 +8334,7 @@
         <v>3.7383E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="10" t="s">
         <v>100</v>
       </c>
@@ -8435,8 +8441,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B87" s="31" t="s">
         <v>102</v>
       </c>
@@ -8474,129 +8480,129 @@
       <c r="AH87" s="31"/>
       <c r="AI87" s="31"/>
     </row>
-    <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B89" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B90" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B91" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B92" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B93" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B94" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="95" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B95" s="11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B96" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B97" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B98" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B99" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B100" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B101" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B102" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B103" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B104" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B105" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B106" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B107" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B108" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B109" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B110" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B111" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="114" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B87:AI87"/>
@@ -8614,18 +8620,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="6" customWidth="1"/>
-    <col min="3" max="37" width="9.140625" style="6"/>
+    <col min="1" max="1" width="20.86328125" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.73046875" style="6" customWidth="1"/>
+    <col min="3" max="37" width="9.1328125" style="6"/>
     <col min="38" max="38" width="8" style="6" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="6"/>
+    <col min="39" max="16384" width="9.1328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C1" s="14">
         <v>2017</v>
@@ -8730,24 +8736,24 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -8755,29 +8761,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="10" t="s">
         <v>9</v>
       </c>
@@ -8785,12 +8791,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
@@ -8897,10 +8903,10 @@
         <v>12</v>
       </c>
       <c r="AK12" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
@@ -9010,18 +9016,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>16</v>
       </c>
@@ -9134,7 +9140,7 @@
         <v>-1.4527999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
@@ -9247,7 +9253,7 @@
         <v>-1.2109E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
@@ -9360,7 +9366,7 @@
         <v>2.2502999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
         <v>22</v>
       </c>
@@ -9473,7 +9479,7 @@
         <v>8.456E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>24</v>
       </c>
@@ -9586,7 +9592,7 @@
         <v>-5.6340000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
         <v>26</v>
       </c>
@@ -9699,7 +9705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
         <v>28</v>
       </c>
@@ -9812,7 +9818,7 @@
         <v>0.123014</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
@@ -9925,7 +9931,7 @@
         <v>5.8900000000000003E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
         <v>32</v>
       </c>
@@ -10038,7 +10044,7 @@
         <v>2.3185000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>34</v>
       </c>
@@ -10151,7 +10157,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="10" t="s">
         <v>37</v>
       </c>
@@ -10264,12 +10270,12 @@
         <v>1.1344E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="10" t="s">
         <v>40</v>
       </c>
@@ -10382,7 +10388,7 @@
         <v>-3.3660000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="10" t="s">
         <v>42</v>
       </c>
@@ -10495,7 +10501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="10" t="s">
         <v>44</v>
       </c>
@@ -10608,7 +10614,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="10" t="s">
         <v>45</v>
       </c>
@@ -10721,7 +10727,7 @@
         <v>-9.68E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="10" t="s">
         <v>46</v>
       </c>
@@ -10834,7 +10840,7 @@
         <v>6.6000000000000005E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="10" t="s">
         <v>47</v>
       </c>
@@ -10947,12 +10953,12 @@
         <v>-4.06E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="10" t="s">
         <v>49</v>
       </c>
@@ -11065,7 +11071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="10" t="s">
         <v>50</v>
       </c>
@@ -11178,7 +11184,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="10" t="s">
         <v>51</v>
       </c>
@@ -11291,7 +11297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="10" t="s">
         <v>52</v>
       </c>
@@ -11404,7 +11410,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="10" t="s">
         <v>53</v>
       </c>
@@ -11517,7 +11523,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="10" t="s">
         <v>55</v>
       </c>
@@ -11630,7 +11636,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="10" t="s">
         <v>56</v>
       </c>
@@ -11743,7 +11749,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
         <v>57</v>
       </c>
@@ -11856,7 +11862,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="10" t="s">
         <v>58</v>
       </c>
@@ -11969,7 +11975,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="10" t="s">
         <v>59</v>
       </c>
@@ -12082,7 +12088,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="10" t="s">
         <v>61</v>
       </c>
@@ -12195,12 +12201,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="10" t="s">
         <v>63</v>
       </c>
@@ -12313,7 +12319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="10" t="s">
         <v>64</v>
       </c>
@@ -12426,7 +12432,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="10" t="s">
         <v>65</v>
       </c>
@@ -12539,7 +12545,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="10" t="s">
         <v>66</v>
       </c>
@@ -12652,7 +12658,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="10" t="s">
         <v>67</v>
       </c>
@@ -12765,7 +12771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="10" t="s">
         <v>68</v>
       </c>
@@ -12878,7 +12884,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="10" t="s">
         <v>69</v>
       </c>
@@ -12991,7 +12997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="10" t="s">
         <v>70</v>
       </c>
@@ -13104,7 +13110,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="10" t="s">
         <v>71</v>
       </c>
@@ -13217,7 +13223,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="10" t="s">
         <v>72</v>
       </c>
@@ -13330,7 +13336,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="10" t="s">
         <v>73</v>
       </c>
@@ -13443,12 +13449,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C60" s="20" t="s">
         <v>36</v>
@@ -13556,12 +13562,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="10" t="s">
         <v>76</v>
       </c>
@@ -13674,7 +13680,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="10" t="s">
         <v>77</v>
       </c>
@@ -13787,7 +13793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="10" t="s">
         <v>78</v>
       </c>
@@ -13900,7 +13906,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="10" t="s">
         <v>79</v>
       </c>
@@ -14013,7 +14019,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="10" t="s">
         <v>80</v>
       </c>
@@ -14126,7 +14132,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="10" t="s">
         <v>81</v>
       </c>
@@ -14239,7 +14245,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="10" t="s">
         <v>82</v>
       </c>
@@ -14352,7 +14358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="10" t="s">
         <v>83</v>
       </c>
@@ -14465,7 +14471,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="10" t="s">
         <v>84</v>
       </c>
@@ -14578,7 +14584,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="10" t="s">
         <v>85</v>
       </c>
@@ -14691,7 +14697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="10" t="s">
         <v>86</v>
       </c>
@@ -14804,12 +14810,12 @@
         <v>1.1053E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B76" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="10" t="s">
         <v>89</v>
       </c>
@@ -14922,7 +14928,7 @@
         <v>-9.3640000000000008E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="10" t="s">
         <v>90</v>
       </c>
@@ -15035,7 +15041,7 @@
         <v>-2.039E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="10" t="s">
         <v>92</v>
       </c>
@@ -15148,7 +15154,7 @@
         <v>2.5253000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="10" t="s">
         <v>94</v>
       </c>
@@ -15261,7 +15267,7 @@
         <v>-7.0799999999999997E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="10" t="s">
         <v>96</v>
       </c>
@@ -15374,7 +15380,7 @@
         <v>6.0502E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="10" t="s">
         <v>97</v>
       </c>
@@ -15487,7 +15493,7 @@
         <v>4.0169999999999997E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="10" t="s">
         <v>99</v>
       </c>
@@ -15600,7 +15606,7 @@
         <v>4.7788999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="10" t="s">
         <v>100</v>
       </c>
@@ -15713,8 +15719,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="87" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B87" s="31" t="s">
         <v>102</v>
       </c>
@@ -15754,139 +15760,139 @@
       <c r="AJ87" s="31"/>
       <c r="AK87" s="31"/>
     </row>
-    <row r="88" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B89" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B90" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B91" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B92" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B93" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B94" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="95" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B95" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="96" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="96" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B96" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B97" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B98" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B99" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B100" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B101" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B102" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B103" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B104" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B105" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B106" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B107" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B108" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B109" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B110" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B111" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="11" t="s">
+    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B112" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="11" t="s">
+    <row r="113" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B113" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="11" t="s">
+    <row r="114" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B114" s="11" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="11" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -15899,28 +15905,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG20"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B2" s="7">
         <v>2035</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -15932,9 +15938,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B4">
         <v>150</v>
@@ -15943,550 +15949,561 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="7" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="6">
+      <c r="B15" s="6">
         <f>'AEO Table 9'!C23</f>
         <v>1.3702000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
-        <v>2019</v>
-      </c>
-      <c r="C14" s="7">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="6">
-        <f>B12</f>
-        <v>1.3702000000000001</v>
-      </c>
-      <c r="C15" s="6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="17" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B17" s="7">
         <v>2019</v>
       </c>
       <c r="C17" s="7">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B15</f>
+        <v>1.3702000000000001</v>
+      </c>
+      <c r="C18" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="B20" s="7">
+        <v>2019</v>
+      </c>
+      <c r="C20" s="7">
         <v>2020</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D20" s="7">
         <v>2021</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E20" s="7">
         <v>2022</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F20" s="7">
         <v>2023</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G20" s="7">
         <v>2024</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H20" s="7">
         <v>2025</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I20" s="7">
         <v>2026</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J20" s="7">
         <v>2027</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K20" s="7">
         <v>2028</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L20" s="7">
         <v>2029</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M20" s="7">
         <v>2030</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N20" s="7">
         <v>2031</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O20" s="7">
         <v>2032</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P20" s="7">
         <v>2033</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q20" s="7">
         <v>2034</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R20" s="7">
         <v>2035</v>
       </c>
-      <c r="S17" s="7">
+      <c r="S20" s="7">
         <v>2036</v>
       </c>
-      <c r="T17" s="7">
+      <c r="T20" s="7">
         <v>2037</v>
       </c>
-      <c r="U17" s="7">
+      <c r="U20" s="7">
         <v>2038</v>
       </c>
-      <c r="V17" s="7">
+      <c r="V20" s="7">
         <v>2039</v>
       </c>
-      <c r="W17" s="7">
+      <c r="W20" s="7">
         <v>2040</v>
       </c>
-      <c r="X17" s="7">
+      <c r="X20" s="7">
         <v>2041</v>
       </c>
-      <c r="Y17" s="7">
+      <c r="Y20" s="7">
         <v>2042</v>
       </c>
-      <c r="Z17" s="7">
+      <c r="Z20" s="7">
         <v>2043</v>
       </c>
-      <c r="AA17" s="7">
+      <c r="AA20" s="7">
         <v>2044</v>
       </c>
-      <c r="AB17" s="7">
+      <c r="AB20" s="7">
         <v>2045</v>
       </c>
-      <c r="AC17" s="7">
+      <c r="AC20" s="7">
         <v>2046</v>
       </c>
-      <c r="AD17" s="7">
+      <c r="AD20" s="7">
         <v>2047</v>
       </c>
-      <c r="AE17" s="7">
+      <c r="AE20" s="7">
         <v>2048</v>
       </c>
-      <c r="AF17" s="7">
+      <c r="AF20" s="7">
         <v>2049</v>
       </c>
-      <c r="AG17" s="7">
+      <c r="AG20" s="7">
         <v>2050</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>176</v>
-      </c>
-      <c r="B18" s="28" cm="1">
-        <f t="array" ref="B18">TREND($B$15:$C$15,$B$14:$C$14,B$17)</f>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="28" cm="1">
+        <f t="array" ref="B21">TREND($B$18:$C$18,$B$17:$C$17,B$20)</f>
         <v>1.3701999999975669</v>
       </c>
-      <c r="C18" s="28" cm="1">
-        <f t="array" ref="C18">TREND($B$15:$C$15,$B$14:$C$14,C$17)</f>
+      <c r="C21" s="28" cm="1">
+        <f t="array" ref="C21">TREND($B$18:$C$18,$B$17:$C$17,C$20)</f>
         <v>17.455032258061692</v>
       </c>
-      <c r="D18" s="28" cm="1">
-        <f t="array" ref="D18">TREND($B$15:$C$15,$B$14:$C$14,D$17)</f>
+      <c r="D21" s="28" cm="1">
+        <f t="array" ref="D21">TREND($B$18:$C$18,$B$17:$C$17,D$20)</f>
         <v>33.539864516125817</v>
       </c>
-      <c r="E18" s="28" cm="1">
-        <f t="array" ref="E18">TREND($B$15:$C$15,$B$14:$C$14,E$17)</f>
+      <c r="E21" s="28" cm="1">
+        <f t="array" ref="E21">TREND($B$18:$C$18,$B$17:$C$17,E$20)</f>
         <v>49.624696774189943</v>
       </c>
-      <c r="F18" s="28" cm="1">
-        <f t="array" ref="F18">TREND($B$15:$C$15,$B$14:$C$14,F$17)</f>
+      <c r="F21" s="28" cm="1">
+        <f t="array" ref="F21">TREND($B$18:$C$18,$B$17:$C$17,F$20)</f>
         <v>65.709529032254068</v>
       </c>
-      <c r="G18" s="28" cm="1">
-        <f t="array" ref="G18">TREND($B$15:$C$15,$B$14:$C$14,G$17)</f>
+      <c r="G21" s="28" cm="1">
+        <f t="array" ref="G21">TREND($B$18:$C$18,$B$17:$C$17,G$20)</f>
         <v>81.794361290318193</v>
       </c>
-      <c r="H18" s="28" cm="1">
-        <f t="array" ref="H18">TREND($B$15:$C$15,$B$14:$C$14,H$17)</f>
+      <c r="H21" s="28" cm="1">
+        <f t="array" ref="H21">TREND($B$18:$C$18,$B$17:$C$17,H$20)</f>
         <v>97.879193548385956</v>
       </c>
-      <c r="I18" s="28" cm="1">
-        <f t="array" ref="I18">TREND($B$15:$C$15,$B$14:$C$14,I$17)</f>
+      <c r="I21" s="28" cm="1">
+        <f t="array" ref="I21">TREND($B$18:$C$18,$B$17:$C$17,I$20)</f>
         <v>113.96402580645008</v>
       </c>
-      <c r="J18" s="28" cm="1">
-        <f t="array" ref="J18">TREND($B$15:$C$15,$B$14:$C$14,J$17)</f>
+      <c r="J21" s="28" cm="1">
+        <f t="array" ref="J21">TREND($B$18:$C$18,$B$17:$C$17,J$20)</f>
         <v>130.04885806451421</v>
       </c>
-      <c r="K18" s="28" cm="1">
-        <f t="array" ref="K18">TREND($B$15:$C$15,$B$14:$C$14,K$17)</f>
+      <c r="K21" s="28" cm="1">
+        <f t="array" ref="K21">TREND($B$18:$C$18,$B$17:$C$17,K$20)</f>
         <v>146.13369032257833</v>
       </c>
-      <c r="L18" s="28" cm="1">
-        <f t="array" ref="L18">TREND($B$15:$C$15,$B$14:$C$14,L$17)</f>
+      <c r="L21" s="28" cm="1">
+        <f t="array" ref="L21">TREND($B$18:$C$18,$B$17:$C$17,L$20)</f>
         <v>162.21852258064246</v>
       </c>
-      <c r="M18" s="28" cm="1">
-        <f t="array" ref="M18">TREND($B$15:$C$15,$B$14:$C$14,M$17)</f>
+      <c r="M21" s="28" cm="1">
+        <f t="array" ref="M21">TREND($B$18:$C$18,$B$17:$C$17,M$20)</f>
         <v>178.30335483870658</v>
       </c>
-      <c r="N18" s="28" cm="1">
-        <f t="array" ref="N18">TREND($B$15:$C$15,$B$14:$C$14,N$17)</f>
+      <c r="N21" s="28" cm="1">
+        <f t="array" ref="N21">TREND($B$18:$C$18,$B$17:$C$17,N$20)</f>
         <v>194.38818709677071</v>
       </c>
-      <c r="O18" s="28" cm="1">
-        <f t="array" ref="O18">TREND($B$15:$C$15,$B$14:$C$14,O$17)</f>
+      <c r="O21" s="28" cm="1">
+        <f t="array" ref="O21">TREND($B$18:$C$18,$B$17:$C$17,O$20)</f>
         <v>210.47301935483483</v>
       </c>
-      <c r="P18" s="28" cm="1">
-        <f t="array" ref="P18">TREND($B$15:$C$15,$B$14:$C$14,P$17)</f>
+      <c r="P21" s="28" cm="1">
+        <f t="array" ref="P21">TREND($B$18:$C$18,$B$17:$C$17,P$20)</f>
         <v>226.55785161289896</v>
       </c>
-      <c r="Q18" s="28" cm="1">
-        <f t="array" ref="Q18">TREND($B$15:$C$15,$B$14:$C$14,Q$17)</f>
+      <c r="Q21" s="28" cm="1">
+        <f t="array" ref="Q21">TREND($B$18:$C$18,$B$17:$C$17,Q$20)</f>
         <v>242.64268387096672</v>
       </c>
-      <c r="R18" s="28" cm="1">
-        <f t="array" ref="R18">TREND($B$15:$C$15,$B$14:$C$14,R$17)</f>
+      <c r="R21" s="28" cm="1">
+        <f t="array" ref="R21">TREND($B$18:$C$18,$B$17:$C$17,R$20)</f>
         <v>258.72751612903085</v>
       </c>
-      <c r="S18" s="28" cm="1">
-        <f t="array" ref="S18">TREND($B$15:$C$15,$B$14:$C$14,S$17)</f>
+      <c r="S21" s="28" cm="1">
+        <f t="array" ref="S21">TREND($B$18:$C$18,$B$17:$C$17,S$20)</f>
         <v>274.81234838709497</v>
       </c>
-      <c r="T18" s="28" cm="1">
-        <f t="array" ref="T18">TREND($B$15:$C$15,$B$14:$C$14,T$17)</f>
+      <c r="T21" s="28" cm="1">
+        <f t="array" ref="T21">TREND($B$18:$C$18,$B$17:$C$17,T$20)</f>
         <v>290.8971806451591</v>
       </c>
-      <c r="U18" s="28" cm="1">
-        <f t="array" ref="U18">TREND($B$15:$C$15,$B$14:$C$14,U$17)</f>
+      <c r="U21" s="28" cm="1">
+        <f t="array" ref="U21">TREND($B$18:$C$18,$B$17:$C$17,U$20)</f>
         <v>306.98201290321958</v>
       </c>
-      <c r="V18" s="28" cm="1">
-        <f t="array" ref="V18">TREND($B$15:$C$15,$B$14:$C$14,V$17)</f>
+      <c r="V21" s="28" cm="1">
+        <f t="array" ref="V21">TREND($B$18:$C$18,$B$17:$C$17,V$20)</f>
         <v>323.06684516129098</v>
       </c>
-      <c r="W18" s="28" cm="1">
-        <f t="array" ref="W18">TREND($B$15:$C$15,$B$14:$C$14,W$17)</f>
+      <c r="W21" s="28" cm="1">
+        <f t="array" ref="W21">TREND($B$18:$C$18,$B$17:$C$17,W$20)</f>
         <v>339.15167741935511</v>
       </c>
-      <c r="X18" s="28" cm="1">
-        <f t="array" ref="X18">TREND($B$15:$C$15,$B$14:$C$14,X$17)</f>
+      <c r="X21" s="28" cm="1">
+        <f t="array" ref="X21">TREND($B$18:$C$18,$B$17:$C$17,X$20)</f>
         <v>355.23650967741924</v>
       </c>
-      <c r="Y18" s="28" cm="1">
-        <f t="array" ref="Y18">TREND($B$15:$C$15,$B$14:$C$14,Y$17)</f>
+      <c r="Y21" s="28" cm="1">
+        <f t="array" ref="Y21">TREND($B$18:$C$18,$B$17:$C$17,Y$20)</f>
         <v>371.32134193548336</v>
       </c>
-      <c r="Z18" s="28" cm="1">
-        <f t="array" ref="Z18">TREND($B$15:$C$15,$B$14:$C$14,Z$17)</f>
+      <c r="Z21" s="28" cm="1">
+        <f t="array" ref="Z21">TREND($B$18:$C$18,$B$17:$C$17,Z$20)</f>
         <v>387.40617419354749</v>
       </c>
-      <c r="AA18" s="28" cm="1">
-        <f t="array" ref="AA18">TREND($B$15:$C$15,$B$14:$C$14,AA$17)</f>
+      <c r="AA21" s="28" cm="1">
+        <f t="array" ref="AA21">TREND($B$18:$C$18,$B$17:$C$17,AA$20)</f>
         <v>403.49100645161161</v>
       </c>
-      <c r="AB18" s="28" cm="1">
-        <f t="array" ref="AB18">TREND($B$15:$C$15,$B$14:$C$14,AB$17)</f>
+      <c r="AB21" s="28" cm="1">
+        <f t="array" ref="AB21">TREND($B$18:$C$18,$B$17:$C$17,AB$20)</f>
         <v>419.57583870967574</v>
       </c>
-      <c r="AC18" s="28" cm="1">
-        <f t="array" ref="AC18">TREND($B$15:$C$15,$B$14:$C$14,AC$17)</f>
+      <c r="AC21" s="28" cm="1">
+        <f t="array" ref="AC21">TREND($B$18:$C$18,$B$17:$C$17,AC$20)</f>
         <v>435.66067096773986</v>
       </c>
-      <c r="AD18" s="28" cm="1">
-        <f t="array" ref="AD18">TREND($B$15:$C$15,$B$14:$C$14,AD$17)</f>
+      <c r="AD21" s="28" cm="1">
+        <f t="array" ref="AD21">TREND($B$18:$C$18,$B$17:$C$17,AD$20)</f>
         <v>451.74550322580399</v>
       </c>
-      <c r="AE18" s="28" cm="1">
-        <f t="array" ref="AE18">TREND($B$15:$C$15,$B$14:$C$14,AE$17)</f>
+      <c r="AE21" s="28" cm="1">
+        <f t="array" ref="AE21">TREND($B$18:$C$18,$B$17:$C$17,AE$20)</f>
         <v>467.83033548386811</v>
       </c>
-      <c r="AF18" s="28" cm="1">
-        <f t="array" ref="AF18">TREND($B$15:$C$15,$B$14:$C$14,AF$17)</f>
+      <c r="AF21" s="28" cm="1">
+        <f t="array" ref="AF21">TREND($B$18:$C$18,$B$17:$C$17,AF$20)</f>
         <v>483.91516774193224</v>
       </c>
-      <c r="AG18" s="28" cm="1">
-        <f t="array" ref="AG18">TREND($B$15:$C$15,$B$14:$C$14,AG$17)</f>
+      <c r="AG21" s="28" cm="1">
+        <f t="array" ref="AG21">TREND($B$18:$C$18,$B$17:$C$17,AG$20)</f>
         <v>499.99999999999636</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" s="28">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="28">
         <f>'AEO Table 9'!C23</f>
         <v>1.3702000000000001</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C22" s="28">
         <f>'AEO Table 9'!D23</f>
         <v>2.62886</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D22" s="28">
         <f>'AEO Table 9'!E23</f>
         <v>5.6288600000000004</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E22" s="28">
         <f>'AEO Table 9'!F23</f>
         <v>6.2598599999999998</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F22" s="28">
         <f>'AEO Table 9'!G23</f>
         <v>6.8908610000000001</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G22" s="28">
         <f>'AEO Table 9'!H23</f>
         <v>7.520861</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H22" s="28">
         <f>'AEO Table 9'!I23</f>
         <v>7.9638609999999996</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I22" s="28">
         <f>'AEO Table 9'!J23</f>
         <v>8.3748609999999992</v>
       </c>
-      <c r="J19" s="28">
+      <c r="J22" s="28">
         <f>'AEO Table 9'!K23</f>
         <v>8.7858610000000006</v>
       </c>
-      <c r="K19" s="28">
+      <c r="K22" s="28">
         <f>'AEO Table 9'!L23</f>
         <v>9.1968610000000002</v>
       </c>
-      <c r="L19" s="28">
+      <c r="L22" s="28">
         <f>'AEO Table 9'!M23</f>
         <v>9.6588419999999999</v>
       </c>
-      <c r="M19" s="28">
+      <c r="M22" s="28">
         <f>'AEO Table 9'!N23</f>
         <v>10.069842</v>
       </c>
-      <c r="N19" s="28">
+      <c r="N22" s="28">
         <f>'AEO Table 9'!O23</f>
         <v>10.069842</v>
       </c>
-      <c r="O19" s="28">
+      <c r="O22" s="28">
         <f>'AEO Table 9'!P23</f>
         <v>10.069842</v>
       </c>
-      <c r="P19" s="28">
+      <c r="P22" s="28">
         <f>'AEO Table 9'!Q23</f>
         <v>10.356866</v>
       </c>
-      <c r="Q19" s="28">
+      <c r="Q22" s="28">
         <f>'AEO Table 9'!R23</f>
         <v>10.804548</v>
       </c>
-      <c r="R19" s="28">
+      <c r="R22" s="28">
         <f>'AEO Table 9'!S23</f>
         <v>10.804548</v>
       </c>
-      <c r="S19" s="28">
+      <c r="S22" s="28">
         <f>'AEO Table 9'!T23</f>
         <v>10.872132000000001</v>
       </c>
-      <c r="T19" s="28">
+      <c r="T22" s="28">
         <f>'AEO Table 9'!U23</f>
         <v>10.872132000000001</v>
       </c>
-      <c r="U19" s="28">
+      <c r="U22" s="28">
         <f>'AEO Table 9'!V23</f>
         <v>10.886932</v>
       </c>
-      <c r="V19" s="28">
+      <c r="V22" s="28">
         <f>'AEO Table 9'!W23</f>
         <v>10.886932</v>
       </c>
-      <c r="W19" s="28">
+      <c r="W22" s="28">
         <f>'AEO Table 9'!X23</f>
         <v>10.974281</v>
       </c>
-      <c r="X19" s="28">
+      <c r="X22" s="28">
         <f>'AEO Table 9'!Y23</f>
         <v>11.413679999999999</v>
       </c>
-      <c r="Y19" s="28">
+      <c r="Y22" s="28">
         <f>'AEO Table 9'!Z23</f>
         <v>12.008404000000001</v>
       </c>
-      <c r="Z19" s="28">
+      <c r="Z22" s="28">
         <f>'AEO Table 9'!AA23</f>
         <v>12.008404000000001</v>
       </c>
-      <c r="AA19" s="28">
+      <c r="AA22" s="28">
         <f>'AEO Table 9'!AB23</f>
         <v>12.008404000000001</v>
       </c>
-      <c r="AB19" s="28">
+      <c r="AB22" s="28">
         <f>'AEO Table 9'!AC23</f>
         <v>12.642261</v>
       </c>
-      <c r="AC19" s="28">
+      <c r="AC22" s="28">
         <f>'AEO Table 9'!AD23</f>
         <v>13.321657</v>
       </c>
-      <c r="AD19" s="28">
+      <c r="AD22" s="28">
         <f>'AEO Table 9'!AE23</f>
         <v>15.081673</v>
       </c>
-      <c r="AE19" s="28">
+      <c r="AE22" s="28">
         <f>'AEO Table 9'!AF23</f>
         <v>16.082681999999998</v>
       </c>
-      <c r="AF19" s="28">
+      <c r="AF22" s="28">
         <f>'AEO Table 9'!AG23</f>
         <v>17.366105999999998</v>
       </c>
-      <c r="AG19" s="28">
+      <c r="AG22" s="28">
         <f>'AEO Table 9'!AH23</f>
         <v>17.400895999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="30">
-        <f>B18-B19</f>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A23" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="30">
+        <f>B21-B22</f>
         <v>-2.4331647807684931E-12</v>
       </c>
-      <c r="C20" s="30">
-        <f t="shared" ref="C20:AG20" si="0">C18-C19</f>
+      <c r="C23" s="30">
+        <f t="shared" ref="C23:AG23" si="0">C21-C22</f>
         <v>14.826172258061693</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D23" s="30">
         <f t="shared" si="0"/>
         <v>27.911004516125818</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E23" s="30">
         <f t="shared" si="0"/>
         <v>43.364836774189939</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F23" s="30">
         <f t="shared" si="0"/>
         <v>58.818668032254067</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G23" s="30">
         <f t="shared" si="0"/>
         <v>74.273500290318196</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H23" s="30">
         <f t="shared" si="0"/>
         <v>89.915332548385962</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I23" s="30">
         <f t="shared" si="0"/>
         <v>105.58916480645009</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J23" s="30">
         <f t="shared" si="0"/>
         <v>121.26299706451421</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K23" s="30">
         <f t="shared" si="0"/>
         <v>136.93682932257832</v>
       </c>
-      <c r="L20" s="30">
+      <c r="L23" s="30">
         <f t="shared" si="0"/>
         <v>152.55968058064246</v>
       </c>
-      <c r="M20" s="30">
+      <c r="M23" s="30">
         <f t="shared" si="0"/>
         <v>168.23351283870659</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N23" s="30">
         <f t="shared" si="0"/>
         <v>184.31834509677071</v>
       </c>
-      <c r="O20" s="30">
+      <c r="O23" s="30">
         <f t="shared" si="0"/>
         <v>200.40317735483484</v>
       </c>
-      <c r="P20" s="30">
+      <c r="P23" s="30">
         <f t="shared" si="0"/>
         <v>216.20098561289896</v>
       </c>
-      <c r="Q20" s="30">
+      <c r="Q23" s="30">
         <f t="shared" si="0"/>
         <v>231.83813587096671</v>
       </c>
-      <c r="R20" s="30">
+      <c r="R23" s="30">
         <f t="shared" si="0"/>
         <v>247.92296812903083</v>
       </c>
-      <c r="S20" s="30">
+      <c r="S23" s="30">
         <f t="shared" si="0"/>
         <v>263.94021638709495</v>
       </c>
-      <c r="T20" s="30">
+      <c r="T23" s="30">
         <f t="shared" si="0"/>
         <v>280.02504864515907</v>
       </c>
-      <c r="U20" s="30">
+      <c r="U23" s="30">
         <f t="shared" si="0"/>
         <v>296.09508090321958</v>
       </c>
-      <c r="V20" s="30">
+      <c r="V23" s="30">
         <f t="shared" si="0"/>
         <v>312.17991316129098</v>
       </c>
-      <c r="W20" s="30">
+      <c r="W23" s="30">
         <f t="shared" si="0"/>
         <v>328.17739641935509</v>
       </c>
-      <c r="X20" s="30">
+      <c r="X23" s="30">
         <f t="shared" si="0"/>
         <v>343.82282967741924</v>
       </c>
-      <c r="Y20" s="30">
+      <c r="Y23" s="30">
         <f t="shared" si="0"/>
         <v>359.31293793548338</v>
       </c>
-      <c r="Z20" s="30">
+      <c r="Z23" s="30">
         <f t="shared" si="0"/>
         <v>375.3977701935475</v>
       </c>
-      <c r="AA20" s="30">
+      <c r="AA23" s="30">
         <f t="shared" si="0"/>
         <v>391.48260245161163</v>
       </c>
-      <c r="AB20" s="30">
+      <c r="AB23" s="30">
         <f t="shared" si="0"/>
         <v>406.93357770967572</v>
       </c>
-      <c r="AC20" s="30">
+      <c r="AC23" s="30">
         <f t="shared" si="0"/>
         <v>422.33901396773985</v>
       </c>
-      <c r="AD20" s="30">
+      <c r="AD23" s="30">
         <f t="shared" si="0"/>
         <v>436.66383022580396</v>
       </c>
-      <c r="AE20" s="30">
+      <c r="AE23" s="30">
         <f t="shared" si="0"/>
         <v>451.74765348386813</v>
       </c>
-      <c r="AF20" s="30">
+      <c r="AF23" s="30">
         <f t="shared" si="0"/>
         <v>466.54906174193223</v>
       </c>
-      <c r="AG20" s="30">
+      <c r="AG23" s="30">
         <f t="shared" si="0"/>
         <v>482.59910399999637</v>
       </c>
@@ -16505,13 +16522,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.1328125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>139</v>
       </c>
@@ -16612,7 +16629,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -16758,16 +16775,16 @@
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="33" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.1328125" customWidth="1"/>
+    <col min="2" max="2" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="33" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>139</v>
       </c>
@@ -16868,136 +16885,136 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>140</v>
       </c>
       <c r="B2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!B20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!B23*gigwatts_to_megawatts</f>
         <v>-2.4331647807684931E-9</v>
       </c>
       <c r="C2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!C20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!C23*gigwatts_to_megawatts</f>
         <v>14826.172258061693</v>
       </c>
       <c r="D2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!D20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!D23*gigwatts_to_megawatts</f>
         <v>27911.004516125817</v>
       </c>
       <c r="E2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!E20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!E23*gigwatts_to_megawatts</f>
         <v>43364.836774189942</v>
       </c>
       <c r="F2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!F20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!F23*gigwatts_to_megawatts</f>
         <v>58818.668032254063</v>
       </c>
       <c r="G2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!G20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!G23*gigwatts_to_megawatts</f>
         <v>74273.500290318203</v>
       </c>
       <c r="H2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!H20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!H23*gigwatts_to_megawatts</f>
         <v>89915.332548385966</v>
       </c>
       <c r="I2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!I20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!I23*gigwatts_to_megawatts</f>
         <v>105589.16480645009</v>
       </c>
       <c r="J2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!J20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!J23*gigwatts_to_megawatts</f>
         <v>121262.99706451422</v>
       </c>
       <c r="K2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!K20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!K23*gigwatts_to_megawatts</f>
         <v>136936.82932257833</v>
       </c>
       <c r="L2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!L20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!L23*gigwatts_to_megawatts</f>
         <v>152559.68058064245</v>
       </c>
       <c r="M2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!M20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!M23*gigwatts_to_megawatts</f>
         <v>168233.51283870658</v>
       </c>
       <c r="N2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!N20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!N23*gigwatts_to_megawatts</f>
         <v>184318.3450967707</v>
       </c>
       <c r="O2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!O20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!O23*gigwatts_to_megawatts</f>
         <v>200403.17735483483</v>
       </c>
       <c r="P2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!P20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!P23*gigwatts_to_megawatts</f>
         <v>216200.98561289895</v>
       </c>
       <c r="Q2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!Q20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!Q23*gigwatts_to_megawatts</f>
         <v>231838.13587096671</v>
       </c>
       <c r="R2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!R20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!R23*gigwatts_to_megawatts</f>
         <v>247922.96812903084</v>
       </c>
       <c r="S2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!S20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!S23*gigwatts_to_megawatts</f>
         <v>263940.21638709493</v>
       </c>
       <c r="T2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!T20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!T23*gigwatts_to_megawatts</f>
         <v>280025.04864515906</v>
       </c>
       <c r="U2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!U20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!U23*gigwatts_to_megawatts</f>
         <v>296095.08090321958</v>
       </c>
       <c r="V2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!V20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!V23*gigwatts_to_megawatts</f>
         <v>312179.91316129098</v>
       </c>
       <c r="W2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!W20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!W23*gigwatts_to_megawatts</f>
         <v>328177.39641935506</v>
       </c>
       <c r="X2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!X20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!X23*gigwatts_to_megawatts</f>
         <v>343822.82967741921</v>
       </c>
       <c r="Y2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!Y20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!Y23*gigwatts_to_megawatts</f>
         <v>359312.93793548335</v>
       </c>
       <c r="Z2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!Z20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!Z23*gigwatts_to_megawatts</f>
         <v>375397.77019354748</v>
       </c>
       <c r="AA2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AA20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!AA23*gigwatts_to_megawatts</f>
         <v>391482.6024516116</v>
       </c>
       <c r="AB2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AB20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!AB23*gigwatts_to_megawatts</f>
         <v>406933.57770967571</v>
       </c>
       <c r="AC2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AC20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!AC23*gigwatts_to_megawatts</f>
         <v>422339.01396773983</v>
       </c>
       <c r="AD2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AD20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!AD23*gigwatts_to_megawatts</f>
         <v>436663.83022580395</v>
       </c>
       <c r="AE2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AE20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!AE23*gigwatts_to_megawatts</f>
         <v>451747.65348386811</v>
       </c>
       <c r="AF2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AF20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!AF23*gigwatts_to_megawatts</f>
         <v>466549.06174193224</v>
       </c>
       <c r="AG2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AG20*gigwatts_to_megawatts</f>
+        <f>'RE Futures Data &amp; Calcs'!AG23*gigwatts_to_megawatts</f>
         <v>482599.10399999638</v>
       </c>
     </row>
@@ -17016,14 +17033,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="11.3984375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>139</v>
       </c>
@@ -17031,16 +17048,16 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" s="5">
         <f>'AEO Table 9 (2019)'!D23*gigwatts_to_megawatts</f>
         <v>752.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B3" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update grid battery storage capacity based on ReEDS data
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\GBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEC742D-2BD5-4C3C-8245-550944F0C0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B76BDA5-6B6E-4B61-B1CD-00B7347D6B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -810,11 +810,13 @@
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="18">
@@ -1656,27 +1658,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="60.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1684,98 +1686,98 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="46" t="s">
         <v>185</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>1000</v>
       </c>
@@ -1797,14 +1799,14 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" customWidth="1"/>
     <col min="38" max="38" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="10" t="s">
         <v>128</v>
       </c>
@@ -1911,8 +1913,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1923,7 +1925,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1936,7 +1938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1947,7 +1949,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1958,7 +1960,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1966,12 +1968,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
@@ -2081,7 +2083,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
@@ -2191,18 +2193,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -2315,7 +2317,7 @@
         <v>-1.4527999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2428,7 +2430,7 @@
         <v>-1.2109E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
@@ -2541,7 +2543,7 @@
         <v>2.2502999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>8.456E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
@@ -2767,7 +2769,7 @@
         <v>-5.6340000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
@@ -2880,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:37" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
         <v>27</v>
       </c>
@@ -2993,7 +2995,7 @@
         <v>0.123014</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -3106,7 +3108,7 @@
         <v>5.8900000000000003E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>31</v>
       </c>
@@ -3219,7 +3221,7 @@
         <v>2.3185000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>33</v>
       </c>
@@ -3332,7 +3334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
@@ -3445,12 +3447,12 @@
         <v>1.1344E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>39</v>
       </c>
@@ -3563,7 +3565,7 @@
         <v>-3.3660000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>41</v>
       </c>
@@ -3676,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>43</v>
       </c>
@@ -3789,7 +3791,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>44</v>
       </c>
@@ -3902,7 +3904,7 @@
         <v>-9.68E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>45</v>
       </c>
@@ -4015,7 +4017,7 @@
         <v>6.6000000000000005E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>46</v>
       </c>
@@ -4128,12 +4130,12 @@
         <v>-4.06E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>48</v>
       </c>
@@ -4246,7 +4248,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>49</v>
       </c>
@@ -4359,7 +4361,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>50</v>
       </c>
@@ -4472,7 +4474,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>51</v>
       </c>
@@ -4585,7 +4587,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>52</v>
       </c>
@@ -4698,7 +4700,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>54</v>
       </c>
@@ -4811,7 +4813,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>55</v>
       </c>
@@ -4924,7 +4926,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>56</v>
       </c>
@@ -5037,7 +5039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>57</v>
       </c>
@@ -5150,7 +5152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>58</v>
       </c>
@@ -5263,7 +5265,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>60</v>
       </c>
@@ -5376,12 +5378,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>62</v>
       </c>
@@ -5494,7 +5496,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>63</v>
       </c>
@@ -5607,7 +5609,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>64</v>
       </c>
@@ -5720,7 +5722,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>65</v>
       </c>
@@ -5833,7 +5835,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>66</v>
       </c>
@@ -5946,7 +5948,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>67</v>
       </c>
@@ -6059,7 +6061,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>68</v>
       </c>
@@ -6172,7 +6174,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>69</v>
       </c>
@@ -6285,7 +6287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>70</v>
       </c>
@@ -6398,7 +6400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>71</v>
       </c>
@@ -6511,7 +6513,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>72</v>
       </c>
@@ -6624,7 +6626,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>73</v>
       </c>
@@ -6737,12 +6739,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>75</v>
       </c>
@@ -6855,7 +6857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>76</v>
       </c>
@@ -6968,7 +6970,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>77</v>
       </c>
@@ -7081,7 +7083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>78</v>
       </c>
@@ -7194,7 +7196,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>79</v>
       </c>
@@ -7307,7 +7309,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>80</v>
       </c>
@@ -7420,7 +7422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>81</v>
       </c>
@@ -7533,7 +7535,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
         <v>82</v>
       </c>
@@ -7646,7 +7648,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>83</v>
       </c>
@@ -7759,7 +7761,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>84</v>
       </c>
@@ -7872,7 +7874,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
         <v>85</v>
       </c>
@@ -7985,12 +7987,12 @@
         <v>1.1053E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
         <v>88</v>
       </c>
@@ -8103,7 +8105,7 @@
         <v>-9.3640000000000008E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
         <v>89</v>
       </c>
@@ -8216,7 +8218,7 @@
         <v>-2.039E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
         <v>91</v>
       </c>
@@ -8329,7 +8331,7 @@
         <v>2.5253000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="7" t="s">
         <v>93</v>
       </c>
@@ -8442,7 +8444,7 @@
         <v>-7.0799999999999997E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>95</v>
       </c>
@@ -8555,7 +8557,7 @@
         <v>6.0502E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
         <v>96</v>
       </c>
@@ -8668,7 +8670,7 @@
         <v>4.0169999999999997E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
         <v>98</v>
       </c>
@@ -8781,7 +8783,7 @@
         <v>4.7788999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
         <v>99</v>
       </c>
@@ -8894,8 +8896,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="87" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="47" t="s">
         <v>101</v>
       </c>
@@ -8935,137 +8937,137 @@
       <c r="AJ87" s="47"/>
       <c r="AK87" s="47"/>
     </row>
-    <row r="88" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B89" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B91" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="92" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B92" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="93" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B93" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B94" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B95" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B96" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B98" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B99" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B100" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B101" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B102" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B105" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B110" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B112" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B113" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B114" s="8" t="s">
         <v>143</v>
       </c>
@@ -9089,14 +9091,14 @@
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="25" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" style="25" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="49" style="25" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="25"/>
+    <col min="3" max="16384" width="9.1796875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="26" t="s">
         <v>174</v>
       </c>
@@ -9191,8 +9193,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
@@ -9203,7 +9205,7 @@
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
     </row>
-    <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="41" t="s">
         <v>4</v>
       </c>
@@ -9216,7 +9218,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="41" t="s">
         <v>6</v>
       </c>
@@ -9227,7 +9229,7 @@
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
     </row>
-    <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="41" t="s">
         <v>7</v>
       </c>
@@ -9238,10 +9240,10 @@
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
     </row>
-    <row r="7" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
         <v>8</v>
       </c>
@@ -9252,7 +9254,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
         <v>10</v>
       </c>
@@ -9260,7 +9262,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="26"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -9296,7 +9298,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="27" t="s">
         <v>12</v>
       </c>
@@ -9394,18 +9396,18 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>15</v>
       </c>
@@ -9506,7 +9508,7 @@
         <v>-2.3927E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
         <v>17</v>
       </c>
@@ -9607,7 +9609,7 @@
         <v>-2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
         <v>19</v>
       </c>
@@ -9708,7 +9710,7 @@
         <v>1.8599000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>21</v>
       </c>
@@ -9809,7 +9811,7 @@
         <v>2.8872999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
         <v>23</v>
       </c>
@@ -9910,7 +9912,7 @@
         <v>-5.8170000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
         <v>25</v>
       </c>
@@ -10011,7 +10013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="28" t="s">
         <v>27</v>
       </c>
@@ -10112,7 +10114,7 @@
         <v>6.9309999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>29</v>
       </c>
@@ -10213,7 +10215,7 @@
         <v>4.9199999999999999E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
         <v>31</v>
       </c>
@@ -10314,7 +10316,7 @@
         <v>3.2424000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
         <v>33</v>
       </c>
@@ -10415,7 +10417,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
         <v>36</v>
       </c>
@@ -10516,12 +10518,12 @@
         <v>1.7170999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
         <v>39</v>
       </c>
@@ -10622,7 +10624,7 @@
         <v>-5.385E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
         <v>41</v>
       </c>
@@ -10723,7 +10725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
         <v>43</v>
       </c>
@@ -10824,7 +10826,7 @@
         <v>-2.9E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>44</v>
       </c>
@@ -10925,7 +10927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
         <v>45</v>
       </c>
@@ -11026,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
         <v>46</v>
       </c>
@@ -11127,13 +11129,13 @@
         <v>-5.3499999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:33" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="B36" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="28" t="s">
         <v>48</v>
       </c>
@@ -11234,7 +11236,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="28" t="s">
         <v>49</v>
       </c>
@@ -11335,7 +11337,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="28" t="s">
         <v>50</v>
       </c>
@@ -11436,7 +11438,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="28" t="s">
         <v>51</v>
       </c>
@@ -11537,7 +11539,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">
         <v>52</v>
       </c>
@@ -11638,7 +11640,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="28" t="s">
         <v>54</v>
       </c>
@@ -11739,7 +11741,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="28" t="s">
         <v>55</v>
       </c>
@@ -11840,7 +11842,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="28" t="s">
         <v>56</v>
       </c>
@@ -11941,7 +11943,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="28" t="s">
         <v>57</v>
       </c>
@@ -12042,7 +12044,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="28" t="s">
         <v>58</v>
       </c>
@@ -12143,7 +12145,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="A47" s="28" t="s">
         <v>60</v>
       </c>
@@ -12244,12 +12246,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="B48" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="28" t="s">
         <v>62</v>
       </c>
@@ -12350,7 +12352,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="28" t="s">
         <v>63</v>
       </c>
@@ -12451,7 +12453,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="28" t="s">
         <v>64</v>
       </c>
@@ -12552,7 +12554,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="28" t="s">
         <v>65</v>
       </c>
@@ -12653,7 +12655,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="28" t="s">
         <v>66</v>
       </c>
@@ -12754,7 +12756,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="28" t="s">
         <v>67</v>
       </c>
@@ -12855,7 +12857,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="28" t="s">
         <v>68</v>
       </c>
@@ -12956,7 +12958,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="28" t="s">
         <v>69</v>
       </c>
@@ -13057,7 +13059,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="28" t="s">
         <v>70</v>
       </c>
@@ -13158,7 +13160,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="58" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="28" t="s">
         <v>71</v>
       </c>
@@ -13259,7 +13261,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="28" t="s">
         <v>72</v>
       </c>
@@ -13360,7 +13362,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="28" t="s">
         <v>73</v>
       </c>
@@ -13461,12 +13463,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="28" t="s">
         <v>75</v>
       </c>
@@ -13567,7 +13569,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="28" t="s">
         <v>76</v>
       </c>
@@ -13668,7 +13670,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="28" t="s">
         <v>77</v>
       </c>
@@ -13769,7 +13771,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" s="28" t="s">
         <v>78</v>
       </c>
@@ -13870,7 +13872,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="28" t="s">
         <v>79</v>
       </c>
@@ -13971,7 +13973,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="28" t="s">
         <v>80</v>
       </c>
@@ -14072,7 +14074,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="28" t="s">
         <v>81</v>
       </c>
@@ -14173,7 +14175,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="70" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="28" t="s">
         <v>82</v>
       </c>
@@ -14274,7 +14276,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="28" t="s">
         <v>83</v>
       </c>
@@ -14375,7 +14377,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="72" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="28" t="s">
         <v>84</v>
       </c>
@@ -14476,8 +14478,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="73" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="28" t="s">
         <v>85</v>
       </c>
@@ -14578,12 +14580,12 @@
         <v>1.6822E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="28" t="s">
         <v>88</v>
       </c>
@@ -14684,7 +14686,7 @@
         <v>-5.5339999999999999E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="28" t="s">
         <v>89</v>
       </c>
@@ -14785,7 +14787,7 @@
         <v>-6.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="28" t="s">
         <v>91</v>
       </c>
@@ -14886,7 +14888,7 @@
         <v>1.1887E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="28" t="s">
         <v>93</v>
       </c>
@@ -14987,7 +14989,7 @@
         <v>5.5900000000000004E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A81" s="28" t="s">
         <v>95</v>
       </c>
@@ -15088,7 +15090,7 @@
         <v>4.9362000000000003E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="28" t="s">
         <v>96</v>
       </c>
@@ -15189,7 +15191,7 @@
         <v>1.895E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="28" t="s">
         <v>98</v>
       </c>
@@ -15290,7 +15292,7 @@
         <v>3.9856000000000003E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="28" t="s">
         <v>99</v>
       </c>
@@ -15391,133 +15393,133 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="38" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="37" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="37" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="37" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="37" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:33" ht="12" x14ac:dyDescent="0.3">
       <c r="B92" s="37" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="37" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="37" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="37" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="97" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="37" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="37" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="37" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="37" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="101" spans="2:33" ht="12" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:33" ht="12" x14ac:dyDescent="0.3">
       <c r="B101" s="37" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="2:33" ht="12" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:33" ht="12" x14ac:dyDescent="0.3">
       <c r="B102" s="37" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="37" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="104" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="37" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="105" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="37" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="106" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="37" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="107" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="37" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="108" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="37" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="109" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="37" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="110" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="37" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="37" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="48"/>
       <c r="C112" s="48"/>
       <c r="D112" s="48"/>
@@ -15551,16 +15553,16 @@
       <c r="AF112" s="48"/>
       <c r="AG112" s="48"/>
     </row>
-    <row r="141" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="12" x14ac:dyDescent="0.2"/>
-    <row r="308" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="142" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="143" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="144" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="308" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B308" s="48"/>
       <c r="C308" s="48"/>
       <c r="D308" s="48"/>
@@ -15594,7 +15596,7 @@
       <c r="AF308" s="48"/>
       <c r="AG308" s="48"/>
     </row>
-    <row r="511" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="511" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B511" s="48"/>
       <c r="C511" s="48"/>
       <c r="D511" s="48"/>
@@ -15628,7 +15630,7 @@
       <c r="AF511" s="48"/>
       <c r="AG511" s="48"/>
     </row>
-    <row r="712" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="712" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B712" s="48"/>
       <c r="C712" s="48"/>
       <c r="D712" s="48"/>
@@ -15662,7 +15664,7 @@
       <c r="AF712" s="48"/>
       <c r="AG712" s="48"/>
     </row>
-    <row r="887" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="887" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B887" s="48"/>
       <c r="C887" s="48"/>
       <c r="D887" s="48"/>
@@ -15696,7 +15698,7 @@
       <c r="AF887" s="48"/>
       <c r="AG887" s="48"/>
     </row>
-    <row r="1100" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1100" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1100" s="48"/>
       <c r="C1100" s="48"/>
       <c r="D1100" s="48"/>
@@ -15730,7 +15732,7 @@
       <c r="AF1100" s="48"/>
       <c r="AG1100" s="48"/>
     </row>
-    <row r="1227" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1227" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1227" s="48"/>
       <c r="C1227" s="48"/>
       <c r="D1227" s="48"/>
@@ -15764,7 +15766,7 @@
       <c r="AF1227" s="48"/>
       <c r="AG1227" s="48"/>
     </row>
-    <row r="1390" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1390" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1390" s="48"/>
       <c r="C1390" s="48"/>
       <c r="D1390" s="48"/>
@@ -15798,7 +15800,7 @@
       <c r="AF1390" s="48"/>
       <c r="AG1390" s="48"/>
     </row>
-    <row r="1502" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1502" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1502" s="48"/>
       <c r="C1502" s="48"/>
       <c r="D1502" s="48"/>
@@ -15832,7 +15834,7 @@
       <c r="AF1502" s="48"/>
       <c r="AG1502" s="48"/>
     </row>
-    <row r="1604" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1604" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1604" s="48"/>
       <c r="C1604" s="48"/>
       <c r="D1604" s="48"/>
@@ -15866,7 +15868,7 @@
       <c r="AF1604" s="48"/>
       <c r="AG1604" s="48"/>
     </row>
-    <row r="1698" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1698" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1698" s="48"/>
       <c r="C1698" s="48"/>
       <c r="D1698" s="48"/>
@@ -15900,7 +15902,7 @@
       <c r="AF1698" s="48"/>
       <c r="AG1698" s="48"/>
     </row>
-    <row r="1945" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1945" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1945" s="48"/>
       <c r="C1945" s="48"/>
       <c r="D1945" s="48"/>
@@ -15934,7 +15936,7 @@
       <c r="AF1945" s="48"/>
       <c r="AG1945" s="48"/>
     </row>
-    <row r="2031" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2031" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2031" s="48"/>
       <c r="C2031" s="48"/>
       <c r="D2031" s="48"/>
@@ -15968,7 +15970,7 @@
       <c r="AF2031" s="48"/>
       <c r="AG2031" s="48"/>
     </row>
-    <row r="2153" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2153" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2153" s="48"/>
       <c r="C2153" s="48"/>
       <c r="D2153" s="48"/>
@@ -16002,7 +16004,7 @@
       <c r="AF2153" s="48"/>
       <c r="AG2153" s="48"/>
     </row>
-    <row r="2317" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2317" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2317" s="48"/>
       <c r="C2317" s="48"/>
       <c r="D2317" s="48"/>
@@ -16036,7 +16038,7 @@
       <c r="AF2317" s="48"/>
       <c r="AG2317" s="48"/>
     </row>
-    <row r="2419" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2419" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2419" s="48"/>
       <c r="C2419" s="48"/>
       <c r="D2419" s="48"/>
@@ -16070,7 +16072,7 @@
       <c r="AF2419" s="48"/>
       <c r="AG2419" s="48"/>
     </row>
-    <row r="2509" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2509" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2509" s="48"/>
       <c r="C2509" s="48"/>
       <c r="D2509" s="48"/>
@@ -16104,7 +16106,7 @@
       <c r="AF2509" s="48"/>
       <c r="AG2509" s="48"/>
     </row>
-    <row r="2598" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2598" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2598" s="48"/>
       <c r="C2598" s="48"/>
       <c r="D2598" s="48"/>
@@ -16138,7 +16140,7 @@
       <c r="AF2598" s="48"/>
       <c r="AG2598" s="48"/>
     </row>
-    <row r="2719" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2719" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2719" s="48"/>
       <c r="C2719" s="48"/>
       <c r="D2719" s="48"/>
@@ -16172,7 +16174,7 @@
       <c r="AF2719" s="48"/>
       <c r="AG2719" s="48"/>
     </row>
-    <row r="2837" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2837" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2837" s="48"/>
       <c r="C2837" s="48"/>
       <c r="D2837" s="48"/>
@@ -16208,14 +16210,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B2719:AG2719"/>
-    <mergeCell ref="B2837:AG2837"/>
-    <mergeCell ref="B2031:AG2031"/>
-    <mergeCell ref="B2153:AG2153"/>
-    <mergeCell ref="B2317:AG2317"/>
-    <mergeCell ref="B2419:AG2419"/>
-    <mergeCell ref="B2509:AG2509"/>
-    <mergeCell ref="B2598:AG2598"/>
     <mergeCell ref="B1945:AG1945"/>
     <mergeCell ref="B112:AG112"/>
     <mergeCell ref="B308:AG308"/>
@@ -16228,6 +16222,14 @@
     <mergeCell ref="B1502:AG1502"/>
     <mergeCell ref="B1604:AG1604"/>
     <mergeCell ref="B1698:AG1698"/>
+    <mergeCell ref="B2719:AG2719"/>
+    <mergeCell ref="B2837:AG2837"/>
+    <mergeCell ref="B2031:AG2031"/>
+    <mergeCell ref="B2153:AG2153"/>
+    <mergeCell ref="B2317:AG2317"/>
+    <mergeCell ref="B2419:AG2419"/>
+    <mergeCell ref="B2509:AG2509"/>
+    <mergeCell ref="B2598:AG2598"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -16245,13 +16247,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>124</v>
       </c>
@@ -16259,7 +16261,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -16268,7 +16270,7 @@
         <v>3968</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
     </row>
   </sheetData>
@@ -16284,14 +16286,16 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>181</v>
       </c>
@@ -16299,12 +16303,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>182</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set GBSC to use an integer value
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B76BDA5-6B6E-4B61-B1CD-00B7347D6B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFA060A-0CE5-4A69-9A11-02A48A4DAA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1662,23 +1662,23 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-    <col min="2" max="2" width="60.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1686,98 +1686,98 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>185</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>1000</v>
       </c>
@@ -1799,14 +1799,14 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" customWidth="1"/>
-    <col min="2" max="2" width="45.7265625" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
     <col min="38" max="38" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
         <v>128</v>
       </c>
@@ -1913,8 +1913,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1925,7 +1925,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1949,7 +1949,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1960,7 +1960,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1968,12 +1968,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
@@ -2193,18 +2193,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>-1.4527999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>-1.2109E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>2.2502999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>8.456E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>-5.6340000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:37" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:37" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>27</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>0.123014</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>5.8900000000000003E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>31</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>2.3185000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>33</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
@@ -3447,12 +3447,12 @@
         <v>1.1344E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>39</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>-3.3660000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>41</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>43</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>44</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>-9.68E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>45</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>6.6000000000000005E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>46</v>
       </c>
@@ -4130,12 +4130,12 @@
         <v>-4.06E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>48</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>49</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>50</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>51</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>52</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>54</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>55</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>56</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>57</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>58</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>60</v>
       </c>
@@ -5378,12 +5378,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>62</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>63</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>64</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>65</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>66</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>67</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>68</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>69</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>70</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>71</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>72</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>73</v>
       </c>
@@ -6739,12 +6739,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>75</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>76</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>77</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>78</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>79</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>80</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>81</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>82</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>83</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>84</v>
       </c>
@@ -7874,7 +7874,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>85</v>
       </c>
@@ -7987,12 +7987,12 @@
         <v>1.1053E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>88</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>-9.3640000000000008E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>89</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>-2.039E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>91</v>
       </c>
@@ -8331,7 +8331,7 @@
         <v>2.5253000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>93</v>
       </c>
@@ -8444,7 +8444,7 @@
         <v>-7.0799999999999997E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>95</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>6.0502E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>96</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>4.0169999999999997E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>98</v>
       </c>
@@ -8783,7 +8783,7 @@
         <v>4.7788999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>99</v>
       </c>
@@ -8896,8 +8896,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="87" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="47" t="s">
         <v>101</v>
       </c>
@@ -8937,137 +8937,137 @@
       <c r="AJ87" s="47"/>
       <c r="AK87" s="47"/>
     </row>
-    <row r="88" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="92" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="93" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="8" t="s">
         <v>143</v>
       </c>
@@ -9091,14 +9091,14 @@
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.453125" style="25" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" style="25" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="49" style="25" customWidth="1"/>
-    <col min="3" max="16384" width="9.1796875" style="25"/>
+    <col min="3" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="26" t="s">
         <v>174</v>
       </c>
@@ -9193,8 +9193,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
@@ -9205,7 +9205,7 @@
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
     </row>
-    <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="41" t="s">
         <v>4</v>
       </c>
@@ -9218,7 +9218,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="41" t="s">
         <v>6</v>
       </c>
@@ -9229,7 +9229,7 @@
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
     </row>
-    <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="41" t="s">
         <v>7</v>
       </c>
@@ -9240,10 +9240,10 @@
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
     </row>
-    <row r="7" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>8</v>
       </c>
@@ -9254,7 +9254,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="26" t="s">
         <v>10</v>
       </c>
@@ -9262,7 +9262,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="26"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -9298,7 +9298,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="27" t="s">
         <v>12</v>
       </c>
@@ -9396,18 +9396,18 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>15</v>
       </c>
@@ -9508,7 +9508,7 @@
         <v>-2.3927E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>17</v>
       </c>
@@ -9609,7 +9609,7 @@
         <v>-2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>19</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>1.8599000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
         <v>21</v>
       </c>
@@ -9811,7 +9811,7 @@
         <v>2.8872999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>23</v>
       </c>
@@ -9912,7 +9912,7 @@
         <v>-5.8170000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>25</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
         <v>27</v>
       </c>
@@ -10114,7 +10114,7 @@
         <v>6.9309999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>29</v>
       </c>
@@ -10215,7 +10215,7 @@
         <v>4.9199999999999999E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>31</v>
       </c>
@@ -10316,7 +10316,7 @@
         <v>3.2424000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>33</v>
       </c>
@@ -10417,7 +10417,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
         <v>36</v>
       </c>
@@ -10518,12 +10518,12 @@
         <v>1.7170999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>39</v>
       </c>
@@ -10624,7 +10624,7 @@
         <v>-5.385E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
         <v>41</v>
       </c>
@@ -10725,7 +10725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>43</v>
       </c>
@@ -10826,7 +10826,7 @@
         <v>-2.9E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>44</v>
       </c>
@@ -10927,7 +10927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>45</v>
       </c>
@@ -11028,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" ht="12" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
         <v>46</v>
       </c>
@@ -11129,13 +11129,13 @@
         <v>-5.3499999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:33" ht="12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:33" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>48</v>
       </c>
@@ -11236,7 +11236,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>49</v>
       </c>
@@ -11337,7 +11337,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>50</v>
       </c>
@@ -11438,7 +11438,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>51</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>52</v>
       </c>
@@ -11640,7 +11640,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>54</v>
       </c>
@@ -11741,7 +11741,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>55</v>
       </c>
@@ -11842,7 +11842,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>56</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>57</v>
       </c>
@@ -12044,7 +12044,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="46" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>58</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" ht="12" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
         <v>60</v>
       </c>
@@ -12246,12 +12246,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:33" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>62</v>
       </c>
@@ -12352,7 +12352,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>63</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>64</v>
       </c>
@@ -12554,7 +12554,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>65</v>
       </c>
@@ -12655,7 +12655,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>66</v>
       </c>
@@ -12756,7 +12756,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>67</v>
       </c>
@@ -12857,7 +12857,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>68</v>
       </c>
@@ -12958,7 +12958,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
         <v>69</v>
       </c>
@@ -13059,7 +13059,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
         <v>70</v>
       </c>
@@ -13160,7 +13160,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="58" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>71</v>
       </c>
@@ -13261,7 +13261,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="28" t="s">
         <v>72</v>
       </c>
@@ -13362,7 +13362,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="28" t="s">
         <v>73</v>
       </c>
@@ -13463,12 +13463,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
         <v>75</v>
       </c>
@@ -13569,7 +13569,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="28" t="s">
         <v>76</v>
       </c>
@@ -13670,7 +13670,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
         <v>77</v>
       </c>
@@ -13771,7 +13771,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="28" t="s">
         <v>78</v>
       </c>
@@ -13872,7 +13872,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="28" t="s">
         <v>79</v>
       </c>
@@ -13973,7 +13973,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
         <v>80</v>
       </c>
@@ -14074,7 +14074,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="28" t="s">
         <v>81</v>
       </c>
@@ -14175,7 +14175,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="70" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="28" t="s">
         <v>82</v>
       </c>
@@ -14276,7 +14276,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="28" t="s">
         <v>83</v>
       </c>
@@ -14377,7 +14377,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="72" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="28" t="s">
         <v>84</v>
       </c>
@@ -14478,8 +14478,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="73" spans="1:33" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:33" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="28" t="s">
         <v>85</v>
       </c>
@@ -14580,12 +14580,12 @@
         <v>1.6822E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
         <v>88</v>
       </c>
@@ -14686,7 +14686,7 @@
         <v>-5.5339999999999999E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="28" t="s">
         <v>89</v>
       </c>
@@ -14787,7 +14787,7 @@
         <v>-6.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="79" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="28" t="s">
         <v>91</v>
       </c>
@@ -14888,7 +14888,7 @@
         <v>1.1887E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="28" t="s">
         <v>93</v>
       </c>
@@ -14989,7 +14989,7 @@
         <v>5.5900000000000004E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" s="28" t="s">
         <v>95</v>
       </c>
@@ -15090,7 +15090,7 @@
         <v>4.9362000000000003E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="28" t="s">
         <v>96</v>
       </c>
@@ -15191,7 +15191,7 @@
         <v>1.895E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="28" t="s">
         <v>98</v>
       </c>
@@ -15292,7 +15292,7 @@
         <v>3.9856000000000003E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="28" t="s">
         <v>99</v>
       </c>
@@ -15393,133 +15393,133 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="87" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="38" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="37" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="37" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="37" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="37" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:33" ht="12" x14ac:dyDescent="0.2">
       <c r="B92" s="37" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="37" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="37" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="37" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="97" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="37" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="37" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="37" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="37" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="101" spans="2:33" ht="12" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:33" ht="12" x14ac:dyDescent="0.2">
       <c r="B101" s="37" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="2:33" ht="12" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:33" ht="12" x14ac:dyDescent="0.2">
       <c r="B102" s="37" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="37" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="104" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="37" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="105" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="37" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="106" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="37" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="107" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="37" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="108" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="37" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="109" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="37" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="110" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="37" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="37" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="48"/>
       <c r="C112" s="48"/>
       <c r="D112" s="48"/>
@@ -15553,16 +15553,16 @@
       <c r="AF112" s="48"/>
       <c r="AG112" s="48"/>
     </row>
-    <row r="141" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="308" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="308" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B308" s="48"/>
       <c r="C308" s="48"/>
       <c r="D308" s="48"/>
@@ -15596,7 +15596,7 @@
       <c r="AF308" s="48"/>
       <c r="AG308" s="48"/>
     </row>
-    <row r="511" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B511" s="48"/>
       <c r="C511" s="48"/>
       <c r="D511" s="48"/>
@@ -15630,7 +15630,7 @@
       <c r="AF511" s="48"/>
       <c r="AG511" s="48"/>
     </row>
-    <row r="712" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="712" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B712" s="48"/>
       <c r="C712" s="48"/>
       <c r="D712" s="48"/>
@@ -15664,7 +15664,7 @@
       <c r="AF712" s="48"/>
       <c r="AG712" s="48"/>
     </row>
-    <row r="887" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="887" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B887" s="48"/>
       <c r="C887" s="48"/>
       <c r="D887" s="48"/>
@@ -15698,7 +15698,7 @@
       <c r="AF887" s="48"/>
       <c r="AG887" s="48"/>
     </row>
-    <row r="1100" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1100" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1100" s="48"/>
       <c r="C1100" s="48"/>
       <c r="D1100" s="48"/>
@@ -15732,7 +15732,7 @@
       <c r="AF1100" s="48"/>
       <c r="AG1100" s="48"/>
     </row>
-    <row r="1227" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1227" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1227" s="48"/>
       <c r="C1227" s="48"/>
       <c r="D1227" s="48"/>
@@ -15766,7 +15766,7 @@
       <c r="AF1227" s="48"/>
       <c r="AG1227" s="48"/>
     </row>
-    <row r="1390" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1390" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1390" s="48"/>
       <c r="C1390" s="48"/>
       <c r="D1390" s="48"/>
@@ -15800,7 +15800,7 @@
       <c r="AF1390" s="48"/>
       <c r="AG1390" s="48"/>
     </row>
-    <row r="1502" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1502" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1502" s="48"/>
       <c r="C1502" s="48"/>
       <c r="D1502" s="48"/>
@@ -15834,7 +15834,7 @@
       <c r="AF1502" s="48"/>
       <c r="AG1502" s="48"/>
     </row>
-    <row r="1604" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1604" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1604" s="48"/>
       <c r="C1604" s="48"/>
       <c r="D1604" s="48"/>
@@ -15868,7 +15868,7 @@
       <c r="AF1604" s="48"/>
       <c r="AG1604" s="48"/>
     </row>
-    <row r="1698" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1698" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1698" s="48"/>
       <c r="C1698" s="48"/>
       <c r="D1698" s="48"/>
@@ -15902,7 +15902,7 @@
       <c r="AF1698" s="48"/>
       <c r="AG1698" s="48"/>
     </row>
-    <row r="1945" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1945" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1945" s="48"/>
       <c r="C1945" s="48"/>
       <c r="D1945" s="48"/>
@@ -15936,7 +15936,7 @@
       <c r="AF1945" s="48"/>
       <c r="AG1945" s="48"/>
     </row>
-    <row r="2031" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2031" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2031" s="48"/>
       <c r="C2031" s="48"/>
       <c r="D2031" s="48"/>
@@ -15970,7 +15970,7 @@
       <c r="AF2031" s="48"/>
       <c r="AG2031" s="48"/>
     </row>
-    <row r="2153" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2153" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2153" s="48"/>
       <c r="C2153" s="48"/>
       <c r="D2153" s="48"/>
@@ -16004,7 +16004,7 @@
       <c r="AF2153" s="48"/>
       <c r="AG2153" s="48"/>
     </row>
-    <row r="2317" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2317" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2317" s="48"/>
       <c r="C2317" s="48"/>
       <c r="D2317" s="48"/>
@@ -16038,7 +16038,7 @@
       <c r="AF2317" s="48"/>
       <c r="AG2317" s="48"/>
     </row>
-    <row r="2419" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2419" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2419" s="48"/>
       <c r="C2419" s="48"/>
       <c r="D2419" s="48"/>
@@ -16072,7 +16072,7 @@
       <c r="AF2419" s="48"/>
       <c r="AG2419" s="48"/>
     </row>
-    <row r="2509" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2509" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2509" s="48"/>
       <c r="C2509" s="48"/>
       <c r="D2509" s="48"/>
@@ -16106,7 +16106,7 @@
       <c r="AF2509" s="48"/>
       <c r="AG2509" s="48"/>
     </row>
-    <row r="2598" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2598" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2598" s="48"/>
       <c r="C2598" s="48"/>
       <c r="D2598" s="48"/>
@@ -16140,7 +16140,7 @@
       <c r="AF2598" s="48"/>
       <c r="AG2598" s="48"/>
     </row>
-    <row r="2719" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2719" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2719" s="48"/>
       <c r="C2719" s="48"/>
       <c r="D2719" s="48"/>
@@ -16174,7 +16174,7 @@
       <c r="AF2719" s="48"/>
       <c r="AG2719" s="48"/>
     </row>
-    <row r="2837" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2837" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2837" s="48"/>
       <c r="C2837" s="48"/>
       <c r="D2837" s="48"/>
@@ -16210,6 +16210,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B2719:AG2719"/>
+    <mergeCell ref="B2837:AG2837"/>
+    <mergeCell ref="B2031:AG2031"/>
+    <mergeCell ref="B2153:AG2153"/>
+    <mergeCell ref="B2317:AG2317"/>
+    <mergeCell ref="B2419:AG2419"/>
+    <mergeCell ref="B2509:AG2509"/>
+    <mergeCell ref="B2598:AG2598"/>
     <mergeCell ref="B1945:AG1945"/>
     <mergeCell ref="B112:AG112"/>
     <mergeCell ref="B308:AG308"/>
@@ -16222,14 +16230,6 @@
     <mergeCell ref="B1502:AG1502"/>
     <mergeCell ref="B1604:AG1604"/>
     <mergeCell ref="B1698:AG1698"/>
-    <mergeCell ref="B2719:AG2719"/>
-    <mergeCell ref="B2837:AG2837"/>
-    <mergeCell ref="B2031:AG2031"/>
-    <mergeCell ref="B2153:AG2153"/>
-    <mergeCell ref="B2317:AG2317"/>
-    <mergeCell ref="B2419:AG2419"/>
-    <mergeCell ref="B2509:AG2509"/>
-    <mergeCell ref="B2598:AG2598"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -16247,13 +16247,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>124</v>
       </c>
@@ -16261,7 +16261,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -16270,7 +16270,7 @@
         <v>3968</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
     </row>
   </sheetData>
@@ -16290,12 +16290,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>181</v>
       </c>
@@ -16303,12 +16303,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>182</v>
       </c>
       <c r="B2">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update battery costs and endo learn parameters, recalibrate against ATB
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFA060A-0CE5-4A69-9A11-02A48A4DAA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B208FE68-64E5-4108-BF53-8E7FAC0EFDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1658,7 +1658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -16210,14 +16210,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B2719:AG2719"/>
-    <mergeCell ref="B2837:AG2837"/>
-    <mergeCell ref="B2031:AG2031"/>
-    <mergeCell ref="B2153:AG2153"/>
-    <mergeCell ref="B2317:AG2317"/>
-    <mergeCell ref="B2419:AG2419"/>
-    <mergeCell ref="B2509:AG2509"/>
-    <mergeCell ref="B2598:AG2598"/>
     <mergeCell ref="B1945:AG1945"/>
     <mergeCell ref="B112:AG112"/>
     <mergeCell ref="B308:AG308"/>
@@ -16230,6 +16222,14 @@
     <mergeCell ref="B1502:AG1502"/>
     <mergeCell ref="B1604:AG1604"/>
     <mergeCell ref="B1698:AG1698"/>
+    <mergeCell ref="B2719:AG2719"/>
+    <mergeCell ref="B2837:AG2837"/>
+    <mergeCell ref="B2031:AG2031"/>
+    <mergeCell ref="B2153:AG2153"/>
+    <mergeCell ref="B2317:AG2317"/>
+    <mergeCell ref="B2419:AG2419"/>
+    <mergeCell ref="B2509:AG2509"/>
+    <mergeCell ref="B2598:AG2598"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -16286,8 +16286,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16308,7 +16308,7 @@
         <v>182</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>